<commit_message>
Add new values (thanks @joel-bourquard)
</commit_message>
<xml_diff>
--- a/decoder.xlsx
+++ b/decoder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyril\Desktop\Arkteos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\arkteos_reg3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A783C675-F6FB-4EA3-B0A2-BA3E513149E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE0D78C-DDF9-4450-937D-9321F93C3F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="32220" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="117">
   <si>
     <t>Donnée</t>
   </si>
@@ -351,6 +351,45 @@
   </si>
   <si>
     <t>3C3</t>
+  </si>
+  <si>
+    <t>fan_speed_evaporator_1</t>
+  </si>
+  <si>
+    <t>Groupe Frigo</t>
+  </si>
+  <si>
+    <t>Voltage DC</t>
+  </si>
+  <si>
+    <t>dc_voltage</t>
+  </si>
+  <si>
+    <t>Voltage DC groupe frigo 1</t>
+  </si>
+  <si>
+    <t>Vitesse ventalisateur groupe frigo 1</t>
+  </si>
+  <si>
+    <t>active_error_reg</t>
+  </si>
+  <si>
+    <t>Erreur active n°1  (régulation)</t>
+  </si>
+  <si>
+    <t>Erreur active n°1 (frigo)</t>
+  </si>
+  <si>
+    <t>Différemment</t>
+  </si>
+  <si>
+    <t>Erreur groupe frigo</t>
+  </si>
+  <si>
+    <t>Erreur régulation</t>
+  </si>
+  <si>
+    <t>&amp; 0x0F</t>
   </si>
 </sst>
 </file>
@@ -687,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,9 +741,9 @@
     <col min="9" max="9" width="6.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.7265625" customWidth="1"/>
-    <col min="19" max="19" width="127.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="70.1796875" customWidth="1"/>
+    <col min="18" max="18" width="70.1796875" customWidth="1"/>
+    <col min="19" max="19" width="32.7265625" customWidth="1"/>
+    <col min="20" max="20" width="127.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -751,13 +790,13 @@
         <v>52</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
@@ -794,15 +833,15 @@
         <v>0</v>
       </c>
       <c r="R2" t="str">
-        <f t="shared" ref="R2:R20" si="0">IF(H2="Oui",_xlfn.CONCAT("        Type number : ",J2," """,K2,"""  [stateTopic=""arkteos/reg3/",J2,"""]"),"")</f>
+        <f t="shared" ref="R2:R23" si="0">IF(H2="Oui",_xlfn.CONCAT("{ 'stream' : ",I2,", 'name' : '",J2,"' ,'descr' : '",K2,"', 'byte1': ",L2,", 'weight1': ",M2,", 'byte2': ",N2,", 'weight2': ",O2,", 'divider': ",P2," }," ),"")</f>
         <v/>
       </c>
       <c r="S2" t="str">
+        <f>IF(H2="Oui",_xlfn.CONCAT("        Type number : ",J2," """,K2,"""  [stateTopic=""arkteos/reg3/",J2,"""]"),"")</f>
+        <v/>
+      </c>
+      <c r="T2" t="str">
         <f>IF(H2="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J2," """,K2,""" {channel=""mqtt:topic:arkteos-reg3:",J2,"""}"),"")</f>
-        <v/>
-      </c>
-      <c r="T2" t="str">
-        <f t="shared" ref="T2:T20" si="1">IF(H2="Oui",_xlfn.CONCAT("{ 'stream' : ",I2,", 'name' : '",J2,"' ,'descr' : '",K2,"', 'byte1': ",L2,", 'weight1': ",M2,", 'byte2': ",N2,", 'weight2': ",O2,", 'divider': ",P2," }," ),"")</f>
         <v/>
       </c>
     </row>
@@ -823,14 +862,14 @@
         <v>68</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I20" si="2">C3</f>
+        <f t="shared" ref="I3:I20" si="1">C3</f>
         <v>227</v>
       </c>
       <c r="J3" t="s">
         <v>70</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K20" si="3">B3</f>
+        <f t="shared" ref="K3:K20" si="2">B3</f>
         <v>Pression eau primaire</v>
       </c>
       <c r="L3">
@@ -849,16 +888,16 @@
         <v>10</v>
       </c>
       <c r="R3" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'primaire_pression' ,'descr' : 'Pression eau primaire', 'byte1': 62, 'weight1': 1, 'byte2': 0, 'weight2': 0, 'divider': 10 },</v>
+      </c>
+      <c r="S3" t="str">
         <f>IF(H3="Oui",_xlfn.CONCAT("        Type number : ",J3," """,K3,"""  [stateTopic=""arkteos/reg3/",J3,"""]"),"")</f>
         <v xml:space="preserve">        Type number : primaire_pression "Pression eau primaire"  [stateTopic="arkteos/reg3/primaire_pression"]</v>
       </c>
-      <c r="S3" t="str">
+      <c r="T3" t="str">
         <f>IF(H3="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J3," """,K3,""" {channel=""mqtt:topic:arkteos-reg3:",J3,"""}"),"")</f>
         <v xml:space="preserve">        Number Arkteosreg3_primaire_pression "Pression eau primaire" {channel="mqtt:topic:arkteos-reg3:primaire_pression"}</v>
-      </c>
-      <c r="T3" t="str">
-        <f t="shared" si="1"/>
-        <v>{ 'stream' : 227, 'name' : 'primaire_pression' ,'descr' : 'Pression eau primaire', 'byte1': 62, 'weight1': 1, 'byte2': 0, 'weight2': 0, 'divider': 10 },</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -878,14 +917,14 @@
         <v>53</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J4" t="s">
         <v>53</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Date année</v>
       </c>
       <c r="R4" t="str">
@@ -893,11 +932,11 @@
         <v/>
       </c>
       <c r="S4" t="str">
-        <f t="shared" ref="S4:S20" si="4">IF(H4="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J4," """,K4,""" {channel=""mqtt:topic:arkteos-reg3:",J4,"""}"),"")</f>
+        <f>IF(H4="Oui",_xlfn.CONCAT("        Type number : ",J4," """,K4,"""  [stateTopic=""arkteos/reg3/",J4,"""]"),"")</f>
         <v/>
       </c>
       <c r="T4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H4="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J4," """,K4,""" {channel=""mqtt:topic:arkteos-reg3:",J4,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -918,14 +957,14 @@
         <v>53</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J5" t="s">
         <v>53</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Date mois</v>
       </c>
       <c r="R5" t="str">
@@ -933,11 +972,11 @@
         <v/>
       </c>
       <c r="S5" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H5="Oui",_xlfn.CONCAT("        Type number : ",J5," """,K5,"""  [stateTopic=""arkteos/reg3/",J5,"""]"),"")</f>
         <v/>
       </c>
       <c r="T5" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H5="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J5," """,K5,""" {channel=""mqtt:topic:arkteos-reg3:",J5,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -958,14 +997,14 @@
         <v>53</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J6" t="s">
         <v>53</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Date jour</v>
       </c>
       <c r="R6" t="str">
@@ -973,11 +1012,11 @@
         <v/>
       </c>
       <c r="S6" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H6="Oui",_xlfn.CONCAT("        Type number : ",J6," """,K6,"""  [stateTopic=""arkteos/reg3/",J6,"""]"),"")</f>
         <v/>
       </c>
       <c r="T6" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H6="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J6," """,K6,""" {channel=""mqtt:topic:arkteos-reg3:",J6,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -998,14 +1037,14 @@
         <v>53</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J7" t="s">
         <v>53</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Date heure</v>
       </c>
       <c r="R7" t="str">
@@ -1013,11 +1052,11 @@
         <v/>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H7="Oui",_xlfn.CONCAT("        Type number : ",J7," """,K7,"""  [stateTopic=""arkteos/reg3/",J7,"""]"),"")</f>
         <v/>
       </c>
       <c r="T7" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H7="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J7," """,K7,""" {channel=""mqtt:topic:arkteos-reg3:",J7,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -1038,14 +1077,14 @@
         <v>53</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J8" t="s">
         <v>53</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Date minutes</v>
       </c>
       <c r="R8" t="str">
@@ -1053,11 +1092,11 @@
         <v/>
       </c>
       <c r="S8" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H8="Oui",_xlfn.CONCAT("        Type number : ",J8," """,K8,"""  [stateTopic=""arkteos/reg3/",J8,"""]"),"")</f>
         <v/>
       </c>
       <c r="T8" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H8="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J8," """,K8,""" {channel=""mqtt:topic:arkteos-reg3:",J8,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -1078,14 +1117,14 @@
         <v>53</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J9" t="s">
         <v>53</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Date secondes</v>
       </c>
       <c r="R9" t="str">
@@ -1093,11 +1132,11 @@
         <v/>
       </c>
       <c r="S9" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H9="Oui",_xlfn.CONCAT("        Type number : ",J9," """,K9,"""  [stateTopic=""arkteos/reg3/",J9,"""]"),"")</f>
         <v/>
       </c>
       <c r="T9" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H9="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J9," """,K9,""" {channel=""mqtt:topic:arkteos-reg3:",J9,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -1118,14 +1157,14 @@
         <v>68</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J10" t="s">
         <v>71</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Température eau primaire aller</v>
       </c>
       <c r="L10">
@@ -1145,15 +1184,15 @@
       </c>
       <c r="R10" t="str">
         <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_aller' ,'descr' : 'Température eau primaire aller', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+      <c r="S10" t="str">
+        <f>IF(H10="Oui",_xlfn.CONCAT("        Type number : ",J10," """,K10,"""  [stateTopic=""arkteos/reg3/",J10,"""]"),"")</f>
         <v xml:space="preserve">        Type number : primaire_temp_eau_aller "Température eau primaire aller"  [stateTopic="arkteos/reg3/primaire_temp_eau_aller"]</v>
       </c>
-      <c r="S10" t="str">
-        <f t="shared" si="4"/>
+      <c r="T10" t="str">
+        <f>IF(H10="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J10," """,K10,""" {channel=""mqtt:topic:arkteos-reg3:",J10,"""}"),"")</f>
         <v xml:space="preserve">        Number Arkteosreg3_primaire_temp_eau_aller "Température eau primaire aller" {channel="mqtt:topic:arkteos-reg3:primaire_temp_eau_aller"}</v>
-      </c>
-      <c r="T10" t="str">
-        <f t="shared" si="1"/>
-        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_aller' ,'descr' : 'Température eau primaire aller', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
@@ -1173,14 +1212,14 @@
         <v>68</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J11" t="s">
         <v>72</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Température eau primaire retour</v>
       </c>
       <c r="L11">
@@ -1200,15 +1239,15 @@
       </c>
       <c r="R11" t="str">
         <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_retour' ,'descr' : 'Température eau primaire retour', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+      <c r="S11" t="str">
+        <f>IF(H11="Oui",_xlfn.CONCAT("        Type number : ",J11," """,K11,"""  [stateTopic=""arkteos/reg3/",J11,"""]"),"")</f>
         <v xml:space="preserve">        Type number : primaire_temp_eau_retour "Température eau primaire retour"  [stateTopic="arkteos/reg3/primaire_temp_eau_retour"]</v>
       </c>
-      <c r="S11" t="str">
-        <f t="shared" si="4"/>
+      <c r="T11" t="str">
+        <f>IF(H11="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J11," """,K11,""" {channel=""mqtt:topic:arkteos-reg3:",J11,"""}"),"")</f>
         <v xml:space="preserve">        Number Arkteosreg3_primaire_temp_eau_retour "Température eau primaire retour" {channel="mqtt:topic:arkteos-reg3:primaire_temp_eau_retour"}</v>
-      </c>
-      <c r="T11" t="str">
-        <f t="shared" si="1"/>
-        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_retour' ,'descr' : 'Température eau primaire retour', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
@@ -1222,14 +1261,14 @@
         <v>227</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J12" t="s">
         <v>73</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Mode zone 1</v>
       </c>
       <c r="R12" t="str">
@@ -1237,17 +1276,17 @@
         <v/>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H12="Oui",_xlfn.CONCAT("        Type number : ",J12," """,K12,"""  [stateTopic=""arkteos/reg3/",J12,"""]"),"")</f>
         <v/>
       </c>
       <c r="T12" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H12="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J12," """,K12,""" {channel=""mqtt:topic:arkteos-reg3:",J12,"""}"),"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -1262,14 +1301,14 @@
         <v>68</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>163</v>
       </c>
       <c r="J13" t="s">
         <v>74</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Température extérieure</v>
       </c>
       <c r="L13">
@@ -1289,15 +1328,15 @@
       </c>
       <c r="R13" t="str">
         <f t="shared" si="0"/>
+        <v>{ 'stream' : 163, 'name' : 'exterieur_temp' ,'descr' : 'Température extérieure', 'byte1': 24, 'weight1': 1, 'byte2': 25, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+      <c r="S13" t="str">
+        <f>IF(H13="Oui",_xlfn.CONCAT("        Type number : ",J13," """,K13,"""  [stateTopic=""arkteos/reg3/",J13,"""]"),"")</f>
         <v xml:space="preserve">        Type number : exterieur_temp "Température extérieure"  [stateTopic="arkteos/reg3/exterieur_temp"]</v>
       </c>
-      <c r="S13" t="str">
-        <f t="shared" si="4"/>
+      <c r="T13" t="str">
+        <f>IF(H13="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J13," """,K13,""" {channel=""mqtt:topic:arkteos-reg3:",J13,"""}"),"")</f>
         <v xml:space="preserve">        Number Arkteosreg3_exterieur_temp "Température extérieure" {channel="mqtt:topic:arkteos-reg3:exterieur_temp"}</v>
-      </c>
-      <c r="T13" t="str">
-        <f t="shared" si="1"/>
-        <v>{ 'stream' : 163, 'name' : 'exterieur_temp' ,'descr' : 'Température extérieure', 'byte1': 24, 'weight1': 1, 'byte2': 25, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
@@ -1317,14 +1356,14 @@
         <v>68</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J14" t="s">
         <v>75</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Température intérieur zone 1</v>
       </c>
       <c r="L14">
@@ -1344,15 +1383,15 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'zone1_temp_interieur' ,'descr' : 'Température intérieur zone 1', 'byte1': 68, 'weight1': 1, 'byte2': 69, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+      <c r="S14" t="str">
+        <f>IF(H14="Oui",_xlfn.CONCAT("        Type number : ",J14," """,K14,"""  [stateTopic=""arkteos/reg3/",J14,"""]"),"")</f>
         <v xml:space="preserve">        Type number : zone1_temp_interieur "Température intérieur zone 1"  [stateTopic="arkteos/reg3/zone1_temp_interieur"]</v>
       </c>
-      <c r="S14" t="str">
-        <f t="shared" si="4"/>
+      <c r="T14" t="str">
+        <f>IF(H14="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J14," """,K14,""" {channel=""mqtt:topic:arkteos-reg3:",J14,"""}"),"")</f>
         <v xml:space="preserve">        Number Arkteosreg3_zone1_temp_interieur "Température intérieur zone 1" {channel="mqtt:topic:arkteos-reg3:zone1_temp_interieur"}</v>
-      </c>
-      <c r="T14" t="str">
-        <f t="shared" si="1"/>
-        <v>{ 'stream' : 227, 'name' : 'zone1_temp_interieur' ,'descr' : 'Température intérieur zone 1', 'byte1': 68, 'weight1': 1, 'byte2': 69, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
@@ -1363,14 +1402,14 @@
         <v>47</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J15" t="s">
         <v>76</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Température eau départ zone 1</v>
       </c>
       <c r="R15" t="str">
@@ -1378,11 +1417,11 @@
         <v/>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H15="Oui",_xlfn.CONCAT("        Type number : ",J15," """,K15,"""  [stateTopic=""arkteos/reg3/",J15,"""]"),"")</f>
         <v/>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H15="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J15," """,K15,""" {channel=""mqtt:topic:arkteos-reg3:",J15,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -1394,14 +1433,14 @@
         <v>48</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>77</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Température eau retour zone 1</v>
       </c>
       <c r="R16" t="str">
@@ -1409,11 +1448,11 @@
         <v/>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H16="Oui",_xlfn.CONCAT("        Type number : ",J16," """,K16,"""  [stateTopic=""arkteos/reg3/",J16,"""]"),"")</f>
         <v/>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H16="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J16," """,K16,""" {channel=""mqtt:topic:arkteos-reg3:",J16,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -1434,14 +1473,14 @@
         <v>68</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J17" t="s">
         <v>78</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Consigne intérieure zone 1</v>
       </c>
       <c r="L17">
@@ -1461,15 +1500,15 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'zone1_consigne' ,'descr' : 'Consigne intérieure zone 1', 'byte1': 70, 'weight1': 1, 'byte2': 71, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+      <c r="S17" t="str">
+        <f>IF(H17="Oui",_xlfn.CONCAT("        Type number : ",J17," """,K17,"""  [stateTopic=""arkteos/reg3/",J17,"""]"),"")</f>
         <v xml:space="preserve">        Type number : zone1_consigne "Consigne intérieure zone 1"  [stateTopic="arkteos/reg3/zone1_consigne"]</v>
       </c>
-      <c r="S17" t="str">
-        <f t="shared" si="4"/>
+      <c r="T17" t="str">
+        <f>IF(H17="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J17," """,K17,""" {channel=""mqtt:topic:arkteos-reg3:",J17,"""}"),"")</f>
         <v xml:space="preserve">        Number Arkteosreg3_zone1_consigne "Consigne intérieure zone 1" {channel="mqtt:topic:arkteos-reg3:zone1_consigne"}</v>
-      </c>
-      <c r="T17" t="str">
-        <f t="shared" si="1"/>
-        <v>{ 'stream' : 227, 'name' : 'zone1_consigne' ,'descr' : 'Consigne intérieure zone 1', 'byte1': 70, 'weight1': 1, 'byte2': 71, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
@@ -1480,14 +1519,14 @@
         <v>8</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J18" t="s">
         <v>79</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Etat (marche)</v>
       </c>
       <c r="R18" t="str">
@@ -1495,11 +1534,11 @@
         <v/>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(H18="Oui",_xlfn.CONCAT("        Type number : ",J18," """,K18,"""  [stateTopic=""arkteos/reg3/",J18,"""]"),"")</f>
         <v/>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(H18="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J18," """,K18,""" {channel=""mqtt:topic:arkteos-reg3:",J18,"""}"),"")</f>
         <v/>
       </c>
     </row>
@@ -1520,14 +1559,14 @@
         <v>68</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J19" t="s">
         <v>80</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Température ballon ECS milieu</v>
       </c>
       <c r="L19">
@@ -1547,15 +1586,15 @@
       </c>
       <c r="R19" t="str">
         <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_milieu' ,'descr' : 'Température ballon ECS milieu', 'byte1': 108, 'weight1': 1, 'byte2': 109, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+      <c r="S19" t="str">
+        <f>IF(H19="Oui",_xlfn.CONCAT("        Type number : ",J19," """,K19,"""  [stateTopic=""arkteos/reg3/",J19,"""]"),"")</f>
         <v xml:space="preserve">        Type number : ecs_temp_eau_milieu "Température ballon ECS milieu"  [stateTopic="arkteos/reg3/ecs_temp_eau_milieu"]</v>
       </c>
-      <c r="S19" t="str">
-        <f t="shared" si="4"/>
+      <c r="T19" t="str">
+        <f>IF(H19="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J19," """,K19,""" {channel=""mqtt:topic:arkteos-reg3:",J19,"""}"),"")</f>
         <v xml:space="preserve">        Number Arkteosreg3_ecs_temp_eau_milieu "Température ballon ECS milieu" {channel="mqtt:topic:arkteos-reg3:ecs_temp_eau_milieu"}</v>
-      </c>
-      <c r="T19" t="str">
-        <f t="shared" si="1"/>
-        <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_milieu' ,'descr' : 'Température ballon ECS milieu', 'byte1': 108, 'weight1': 1, 'byte2': 109, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
@@ -1575,14 +1614,14 @@
         <v>68</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="J20" t="s">
         <v>81</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Température ballon ECS bas</v>
       </c>
       <c r="L20">
@@ -1602,31 +1641,179 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_bas' ,'descr' : 'Température ballon ECS bas', 'byte1': 110, 'weight1': 1, 'byte2': 111, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+      <c r="S20" t="str">
+        <f>IF(H20="Oui",_xlfn.CONCAT("        Type number : ",J20," """,K20,"""  [stateTopic=""arkteos/reg3/",J20,"""]"),"")</f>
         <v xml:space="preserve">        Type number : ecs_temp_eau_bas "Température ballon ECS bas"  [stateTopic="arkteos/reg3/ecs_temp_eau_bas"]</v>
       </c>
-      <c r="S20" t="str">
-        <f t="shared" si="4"/>
+      <c r="T20" t="str">
+        <f>IF(H20="Oui",_xlfn.CONCAT("        Number Arkteosreg3_",J20," """,K20,""" {channel=""mqtt:topic:arkteos-reg3:",J20,"""}"),"")</f>
         <v xml:space="preserve">        Number Arkteosreg3_ecs_temp_eau_bas "Température ballon ECS bas" {channel="mqtt:topic:arkteos-reg3:ecs_temp_eau_bas"}</v>
       </c>
-      <c r="T20" t="str">
-        <f t="shared" si="1"/>
-        <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_bas' ,'descr' : 'Température ballon ECS bas', 'byte1': 110, 'weight1': 1, 'byte2': 111, 'weight2': 256, 'divider': 10 },</v>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21">
+        <v>163</v>
+      </c>
+      <c r="J21" t="s">
+        <v>104</v>
+      </c>
+      <c r="K21" t="s">
+        <v>109</v>
+      </c>
+      <c r="L21">
+        <v>56</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>57</v>
+      </c>
+      <c r="O21">
+        <v>256</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="R21" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 163, 'name' : 'fan_speed_evaporator_1' ,'descr' : 'Vitesse ventalisateur groupe frigo 1', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 1 },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22">
+        <v>163</v>
+      </c>
+      <c r="H22" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22">
+        <v>163</v>
+      </c>
+      <c r="J22" t="s">
+        <v>107</v>
+      </c>
+      <c r="K22" t="s">
+        <v>108</v>
+      </c>
+      <c r="L22">
+        <v>62</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>63</v>
+      </c>
+      <c r="O22">
+        <v>256</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="R22" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 163, 'name' : 'dc_voltage' ,'descr' : 'Voltage DC groupe frigo 1', 'byte1': 62, 'weight1': 1, 'byte2': 63, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>111</v>
+      </c>
+      <c r="C23">
+        <v>227</v>
+      </c>
+      <c r="H23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23">
+        <v>227</v>
+      </c>
+      <c r="J23" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" t="s">
+        <v>115</v>
+      </c>
+      <c r="L23">
+        <v>30</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>31</v>
+      </c>
+      <c r="O23">
+        <v>256</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>116</v>
+      </c>
+      <c r="R23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>112</v>
+      </c>
+      <c r="C24">
+        <v>163</v>
+      </c>
+      <c r="H24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24">
+        <v>163</v>
+      </c>
+      <c r="K24" t="s">
+        <v>114</v>
+      </c>
+      <c r="L24">
+        <v>12</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>13</v>
+      </c>
+      <c r="O24">
+        <v>256</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
@@ -1634,28 +1821,28 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
@@ -1663,9 +1850,17 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
         <v>91</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add PAC status + manage new MQTT API version management
</commit_message>
<xml_diff>
--- a/decoder.xlsx
+++ b/decoder.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\arkteos_reg3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4F32B9-AAB0-4971-A00F-63D98B68580E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968228D4-0547-4568-AC64-1DB39637BAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="90" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
     <sheet name="Struct" sheetId="5" r:id="rId2"/>
-    <sheet name="S_CYCL_REG_FRI" sheetId="6" r:id="rId3"/>
-    <sheet name="S_CYCLIQUE_ETHER_REG_REGUL_T1" sheetId="7" r:id="rId4"/>
+    <sheet name="S_CYCLIQUE_ETHER_REG_REGUL_T1" sheetId="7" r:id="rId3"/>
+    <sheet name="S_CYCL_REG_FRI" sheetId="6" r:id="rId4"/>
     <sheet name="Lower_case" sheetId="3" r:id="rId5"/>
     <sheet name="Simul" sheetId="2" r:id="rId6"/>
     <sheet name="Histo" sheetId="4" r:id="rId7"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="250">
   <si>
     <t>Donnée</t>
   </si>
@@ -783,6 +783,15 @@
   </si>
   <si>
     <t>u16NbDegivrage</t>
+  </si>
+  <si>
+    <t>Statut PAC</t>
+  </si>
+  <si>
+    <t>Mode PAC</t>
+  </si>
+  <si>
+    <t>statut_pac</t>
   </si>
 </sst>
 </file>
@@ -904,24 +913,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -932,6 +932,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1214,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1372,7 @@
         <v>10</v>
       </c>
       <c r="Q3" t="str">
-        <f>IF(G3="Oui",_xlfn.CONCAT("{ 'stream' : ",H3,", 'name' : '",I3,"' ,'descr' : '",J3,"', 'byte1': ",K3,", 'weight1': ",L3,", 'byte2': ",M3,", 'weight2': ",N3,", 'divider': ",O3," }," ),"")</f>
+        <f t="shared" ref="Q3:Q22" si="0">IF(G3="Oui",_xlfn.CONCAT("{ 'stream' : ",H3,", 'name' : '",I3,"' ,'descr' : '",J3,"', 'byte1': ",K3,", 'weight1': ",L3,", 'byte2': ",M3,", 'weight2': ",N3,", 'divider': ",O3," }," ),"")</f>
         <v>{ 'stream' : 163, 'name' : 'exterieur_temp' ,'descr' : 'Température extérieure', 'byte1': 24, 'weight1': 1, 'byte2': 25, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
@@ -1374,7 +1380,7 @@
       <c r="A4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C4">
@@ -1408,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="str">
-        <f>IF(G4="Oui",_xlfn.CONCAT("{ 'stream' : ",H4,", 'name' : '",I4,"' ,'descr' : '",J4,"', 'byte1': ",K4,", 'weight1': ",L4,", 'byte2': ",M4,", 'weight2': ",N4,", 'divider': ",O4," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v>{ 'stream' : 163, 'name' : 'freq_comp_actuelle' ,'descr' : 'Fréquence compresseur actuelle', 'byte1': 52, 'weight1': 1, 'byte2': 53, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
@@ -1416,7 +1422,7 @@
       <c r="A5" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>138</v>
       </c>
       <c r="C5">
@@ -1450,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="Q5" t="str">
-        <f>IF(G5="Oui",_xlfn.CONCAT("{ 'stream' : ",H5,", 'name' : '",I5,"' ,'descr' : '",J5,"', 'byte1': ",K5,", 'weight1': ",L5,", 'byte2': ",M5,", 'weight2': ",N5,", 'divider': ",O5," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v>{ 'stream' : 163, 'name' : 'freq_comp_cible' ,'descr' : 'Fréquence compresseur cible', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
@@ -1492,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="Q6" t="str">
-        <f>IF(G6="Oui",_xlfn.CONCAT("{ 'stream' : ",H6,", 'name' : '",I6,"' ,'descr' : '",J6,"', 'byte1': ",K6,", 'weight1': ",L6,", 'byte2': ",M6,", 'weight2': ",N6,", 'divider': ",O6," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v>{ 'stream' : 163, 'name' : 'fan_speed_evaporator_1' ,'descr' : 'Vitesse ventalisateur groupe frigo 1', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
@@ -1534,137 +1540,125 @@
         <v>1</v>
       </c>
       <c r="Q7" t="str">
-        <f>IF(G7="Oui",_xlfn.CONCAT("{ 'stream' : ",H7,", 'name' : '",I7,"' ,'descr' : '",J7,"', 'byte1': ",K7,", 'weight1': ",L7,", 'byte2': ",M7,", 'weight2': ",N7,", 'divider': ",O7," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v>{ 'stream' : 163, 'name' : 'dc_voltage' ,'descr' : 'Voltage DC groupe frigo 1', 'byte1': 62, 'weight1': 1, 'byte2': 63, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>248</v>
       </c>
       <c r="C8">
         <v>227</v>
       </c>
-      <c r="G8" t="s">
-        <v>111</v>
-      </c>
       <c r="H8">
         <v>227</v>
       </c>
       <c r="I8" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>248</v>
       </c>
       <c r="K8">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>1</v>
       </c>
-      <c r="P8" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q8" t="str">
-        <f>IF(G8="Oui",_xlfn.CONCAT("{ 'stream' : ",H8,", 'name' : '",I8,"' ,'descr' : '",J8,"', 'byte1': ",K8,", 'weight1': ",L8,", 'byte2': ",M8,", 'weight2': ",N8,", 'divider': ",O8," }," ),"")</f>
-        <v/>
-      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>227</v>
       </c>
-      <c r="E9">
-        <v>54.55</v>
-      </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="H9">
-        <f>C9</f>
         <v>227</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" t="str">
-        <f>B9</f>
-        <v>Température eau primaire aller</v>
+        <v>108</v>
+      </c>
+      <c r="J9" t="s">
+        <v>113</v>
       </c>
       <c r="K9">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="N9">
         <v>256</v>
       </c>
       <c r="O9">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>114</v>
       </c>
       <c r="Q9" t="str">
-        <f>IF(G9="Oui",_xlfn.CONCAT("{ 'stream' : ",H9,", 'name' : '",I9,"' ,'descr' : '",J9,"', 'byte1': ",K9,", 'weight1': ",L9,", 'byte2': ",M9,", 'weight2': ",N9,", 'divider': ",O9," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_aller' ,'descr' : 'Température eau primaire aller', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 10 },</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>227</v>
       </c>
       <c r="E10">
-        <v>56.57</v>
+        <v>54.55</v>
       </c>
       <c r="G10" t="s">
         <v>68</v>
       </c>
       <c r="H10">
-        <f>C10</f>
+        <f t="shared" ref="H10:H28" si="1">C10</f>
         <v>227</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10" t="str">
-        <f>B10</f>
-        <v>Température eau primaire retour</v>
+        <f t="shared" ref="J10:J22" si="2">B10</f>
+        <v>Température eau primaire aller</v>
       </c>
       <c r="K10">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N10">
         <v>256</v>
@@ -1673,102 +1667,102 @@
         <v>10</v>
       </c>
       <c r="Q10" t="str">
-        <f>IF(G10="Oui",_xlfn.CONCAT("{ 'stream' : ",H10,", 'name' : '",I10,"' ,'descr' : '",J10,"', 'byte1': ",K10,", 'weight1': ",L10,", 'byte2': ",M10,", 'weight2': ",N10,", 'divider': ",O10," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_retour' ,'descr' : 'Température eau primaire retour', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 10 },</v>
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_aller' ,'descr' : 'Température eau primaire aller', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>227</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
+      <c r="E11">
+        <v>56.57</v>
       </c>
       <c r="G11" t="s">
         <v>68</v>
       </c>
       <c r="H11">
-        <f>C11</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J11" t="str">
-        <f>B11</f>
-        <v>Pression eau primaire</v>
+        <f t="shared" si="2"/>
+        <v>Température eau primaire retour</v>
       </c>
       <c r="K11">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="O11">
         <v>10</v>
       </c>
       <c r="Q11" t="str">
-        <f>IF(G11="Oui",_xlfn.CONCAT("{ 'stream' : ",H11,", 'name' : '",I11,"' ,'descr' : '",J11,"', 'byte1': ",K11,", 'weight1': ",L11,", 'byte2': ",M11,", 'weight2': ",N11,", 'divider': ",O11," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'primaire_pression' ,'descr' : 'Pression eau primaire', 'byte1': 62, 'weight1': 1, 'byte2': 0, 'weight2': 0, 'divider': 10 },</v>
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_retour' ,'descr' : 'Température eau primaire retour', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>247</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C12">
         <v>227</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G12" t="s">
         <v>68</v>
       </c>
       <c r="H12">
-        <f>C12</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J12" t="str">
-        <f>B12</f>
-        <v>Température intérieur zone 1</v>
+        <f t="shared" si="2"/>
+        <v>Pression eau primaire</v>
       </c>
       <c r="K12">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>10</v>
       </c>
       <c r="Q12" t="str">
-        <f>IF(G12="Oui",_xlfn.CONCAT("{ 'stream' : ",H12,", 'name' : '",I12,"' ,'descr' : '",J12,"', 'byte1': ",K12,", 'weight1': ",L12,", 'byte2': ",M12,", 'weight2': ",N12,", 'divider': ",O12," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'zone1_temp_interieur' ,'descr' : 'Température intérieur zone 1', 'byte1': 68, 'weight1': 1, 'byte2': 69, 'weight2': 256, 'divider': 10 },</v>
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'primaire_pression' ,'descr' : 'Pression eau primaire', 'byte1': 62, 'weight1': 1, 'byte2': 0, 'weight2': 0, 'divider': 10 },</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1776,36 +1770,36 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>227</v>
       </c>
-      <c r="E13">
-        <v>70.709999999999994</v>
+      <c r="D13" t="s">
+        <v>26</v>
       </c>
       <c r="G13" t="s">
         <v>68</v>
       </c>
       <c r="H13">
-        <f>C13</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J13" t="str">
-        <f>B13</f>
-        <v>Consigne intérieure zone 1</v>
+        <f t="shared" si="2"/>
+        <v>Température intérieur zone 1</v>
       </c>
       <c r="K13">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
       <c r="M13">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N13">
         <v>256</v>
@@ -1814,45 +1808,45 @@
         <v>10</v>
       </c>
       <c r="Q13" t="str">
-        <f>IF(G13="Oui",_xlfn.CONCAT("{ 'stream' : ",H13,", 'name' : '",I13,"' ,'descr' : '",J13,"', 'byte1': ",K13,", 'weight1': ",L13,", 'byte2': ",M13,", 'weight2': ",N13,", 'divider': ",O13," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'zone1_consigne' ,'descr' : 'Consigne intérieure zone 1', 'byte1': 70, 'weight1': 1, 'byte2': 71, 'weight2': 256, 'divider': 10 },</v>
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'zone1_temp_interieur' ,'descr' : 'Température intérieur zone 1', 'byte1': 68, 'weight1': 1, 'byte2': 69, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>227</v>
       </c>
-      <c r="D14" t="s">
-        <v>11</v>
+      <c r="E14">
+        <v>70.709999999999994</v>
       </c>
       <c r="G14" t="s">
         <v>68</v>
       </c>
       <c r="H14">
-        <f>C14</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J14" t="str">
-        <f>B14</f>
-        <v>Température ballon ECS milieu</v>
+        <f t="shared" si="2"/>
+        <v>Consigne intérieure zone 1</v>
       </c>
       <c r="K14">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="L14">
         <v>1</v>
       </c>
       <c r="M14">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="N14">
         <v>256</v>
@@ -1861,8 +1855,8 @@
         <v>10</v>
       </c>
       <c r="Q14" t="str">
-        <f>IF(G14="Oui",_xlfn.CONCAT("{ 'stream' : ",H14,", 'name' : '",I14,"' ,'descr' : '",J14,"', 'byte1': ",K14,", 'weight1': ",L14,", 'byte2': ",M14,", 'weight2': ",N14,", 'divider': ",O14," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_milieu' ,'descr' : 'Température ballon ECS milieu', 'byte1': 108, 'weight1': 1, 'byte2': 109, 'weight2': 256, 'divider': 10 },</v>
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'zone1_consigne' ,'descr' : 'Consigne intérieure zone 1', 'byte1': 70, 'weight1': 1, 'byte2': 71, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1870,36 +1864,36 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>227</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
         <v>68</v>
       </c>
       <c r="H15">
-        <f>C15</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J15" t="str">
-        <f>B15</f>
-        <v>Température ballon ECS bas</v>
+        <f t="shared" si="2"/>
+        <v>Température ballon ECS milieu</v>
       </c>
       <c r="K15">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L15">
         <v>1</v>
       </c>
       <c r="M15">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N15">
         <v>256</v>
@@ -1908,40 +1902,55 @@
         <v>10</v>
       </c>
       <c r="Q15" t="str">
-        <f>IF(G15="Oui",_xlfn.CONCAT("{ 'stream' : ",H15,", 'name' : '",I15,"' ,'descr' : '",J15,"', 'byte1': ",K15,", 'weight1': ",L15,", 'byte2': ",M15,", 'weight2': ",N15,", 'divider': ",O15," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_bas' ,'descr' : 'Température ballon ECS bas', 'byte1': 110, 'weight1': 1, 'byte2': 111, 'weight2': 256, 'divider': 10 },</v>
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_milieu' ,'descr' : 'Température ballon ECS milieu', 'byte1': 108, 'weight1': 1, 'byte2': 109, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>227</v>
       </c>
-      <c r="E16">
-        <v>168</v>
+      <c r="D16" t="s">
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H16">
-        <f>C16</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I16" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="J16" t="str">
-        <f>B16</f>
-        <v>Date année</v>
+        <f t="shared" si="2"/>
+        <v>Température ballon ECS bas</v>
+      </c>
+      <c r="K16">
+        <v>110</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>111</v>
+      </c>
+      <c r="N16">
+        <v>256</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
       </c>
       <c r="Q16" t="str">
-        <f>IF(G16="Oui",_xlfn.CONCAT("{ 'stream' : ",H16,", 'name' : '",I16,"' ,'descr' : '",J16,"', 'byte1': ",K16,", 'weight1': ",L16,", 'byte2': ",M16,", 'weight2': ",N16,", 'divider': ",O16," }," ),"")</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_bas' ,'descr' : 'Température ballon ECS bas', 'byte1': 110, 'weight1': 1, 'byte2': 111, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1949,30 +1958,30 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>227</v>
       </c>
       <c r="E17">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G17" t="s">
         <v>53</v>
       </c>
       <c r="H17">
-        <f>C17</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I17" t="s">
         <v>53</v>
       </c>
       <c r="J17" t="str">
-        <f>B17</f>
-        <v>Date mois</v>
+        <f t="shared" si="2"/>
+        <v>Date année</v>
       </c>
       <c r="Q17" t="str">
-        <f>IF(G17="Oui",_xlfn.CONCAT("{ 'stream' : ",H17,", 'name' : '",I17,"' ,'descr' : '",J17,"', 'byte1': ",K17,", 'weight1': ",L17,", 'byte2': ",M17,", 'weight2': ",N17,", 'divider': ",O17," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1981,30 +1990,30 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>227</v>
       </c>
       <c r="E18">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G18" t="s">
         <v>53</v>
       </c>
       <c r="H18">
-        <f>C18</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I18" t="s">
         <v>53</v>
       </c>
       <c r="J18" t="str">
-        <f>B18</f>
-        <v>Date jour</v>
+        <f t="shared" si="2"/>
+        <v>Date mois</v>
       </c>
       <c r="Q18" t="str">
-        <f>IF(G18="Oui",_xlfn.CONCAT("{ 'stream' : ",H18,", 'name' : '",I18,"' ,'descr' : '",J18,"', 'byte1': ",K18,", 'weight1': ",L18,", 'byte2': ",M18,", 'weight2': ",N18,", 'divider': ",O18," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2013,30 +2022,30 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>227</v>
       </c>
       <c r="E19">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G19" t="s">
         <v>53</v>
       </c>
       <c r="H19">
-        <f>C19</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I19" t="s">
         <v>53</v>
       </c>
       <c r="J19" t="str">
-        <f>B19</f>
-        <v>Date heure</v>
+        <f t="shared" si="2"/>
+        <v>Date jour</v>
       </c>
       <c r="Q19" t="str">
-        <f>IF(G19="Oui",_xlfn.CONCAT("{ 'stream' : ",H19,", 'name' : '",I19,"' ,'descr' : '",J19,"', 'byte1': ",K19,", 'weight1': ",L19,", 'byte2': ",M19,", 'weight2': ",N19,", 'divider': ",O19," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2045,30 +2054,30 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>227</v>
       </c>
       <c r="E20">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G20" t="s">
         <v>53</v>
       </c>
       <c r="H20">
-        <f>C20</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I20" t="s">
         <v>53</v>
       </c>
       <c r="J20" t="str">
-        <f>B20</f>
-        <v>Date minutes</v>
+        <f t="shared" si="2"/>
+        <v>Date heure</v>
       </c>
       <c r="Q20" t="str">
-        <f>IF(G20="Oui",_xlfn.CONCAT("{ 'stream' : ",H20,", 'name' : '",I20,"' ,'descr' : '",J20,"', 'byte1': ",K20,", 'weight1': ",L20,", 'byte2': ",M20,", 'weight2': ",N20,", 'divider': ",O20," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2077,30 +2086,30 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>227</v>
       </c>
       <c r="E21">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G21" t="s">
         <v>53</v>
       </c>
       <c r="H21">
-        <f>C21</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I21" t="s">
         <v>53</v>
       </c>
       <c r="J21" t="str">
-        <f>B21</f>
-        <v>Date secondes</v>
+        <f t="shared" si="2"/>
+        <v>Date minutes</v>
       </c>
       <c r="Q21" t="str">
-        <f>IF(G21="Oui",_xlfn.CONCAT("{ 'stream' : ",H21,", 'name' : '",I21,"' ,'descr' : '",J21,"', 'byte1': ",K21,", 'weight1': ",L21,", 'byte2': ",M21,", 'weight2': ",N21,", 'divider': ",O21," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2109,89 +2118,83 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="C22">
         <v>227</v>
       </c>
+      <c r="E22">
+        <v>173</v>
+      </c>
       <c r="G22" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="H22">
-        <f>C22</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J22" t="s">
-        <v>143</v>
-      </c>
-      <c r="K22">
-        <v>193</v>
-      </c>
-      <c r="L22">
-        <v>1</v>
+      <c r="I22" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="2"/>
+        <v>Date secondes</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>143</v>
       </c>
       <c r="C23">
         <v>227</v>
       </c>
+      <c r="G23" t="s">
+        <v>111</v>
+      </c>
       <c r="H23">
-        <f>C23</f>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I23" t="s">
-        <v>73</v>
-      </c>
-      <c r="J23" t="str">
-        <f>B23</f>
-        <v>Mode zone 1</v>
-      </c>
-      <c r="Q23" t="str">
-        <f>IF(G23="Oui",_xlfn.CONCAT("{ 'stream' : ",H23,", 'name' : '",I23,"' ,'descr' : '",J23,"', 'byte1': ",K23,", 'weight1': ",L23,", 'byte2': ",M23,", 'weight2': ",N23,", 'divider': ",O23," }," ),"")</f>
-        <v/>
+        <v>144</v>
+      </c>
+      <c r="J23" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23">
+        <v>193</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="C24">
+        <v>227</v>
       </c>
       <c r="H24">
-        <f>C24</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>227</v>
       </c>
       <c r="I24" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J24" t="str">
         <f>B24</f>
-        <v>Marche/Arrêt Général</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
+        <v>Mode zone 1</v>
       </c>
       <c r="Q24" t="str">
         <f>IF(G24="Oui",_xlfn.CONCAT("{ 'stream' : ",H24,", 'name' : '",I24,"' ,'descr' : '",J24,"', 'byte1': ",K24,", 'weight1': ",L24,", 'byte2': ",M24,", 'weight2': ",N24,", 'divider': ",O24," }," ),"")</f>
@@ -2200,21 +2203,36 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H25">
-        <f>C25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="J25" t="str">
         <f>B25</f>
-        <v>Température eau départ zone 1</v>
+        <v>Marche/Arrêt Général</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
       </c>
       <c r="Q25" t="str">
         <f>IF(G25="Oui",_xlfn.CONCAT("{ 'stream' : ",H25,", 'name' : '",I25,"' ,'descr' : '",J25,"', 'byte1': ",K25,", 'weight1': ",L25,", 'byte2': ",M25,", 'weight2': ",N25,", 'divider': ",O25," }," ),"")</f>
@@ -2226,18 +2244,18 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H26">
-        <f>C26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J26" t="str">
         <f>B26</f>
-        <v>Température eau retour zone 1</v>
+        <v>Température eau départ zone 1</v>
       </c>
       <c r="Q26" t="str">
         <f>IF(G26="Oui",_xlfn.CONCAT("{ 'stream' : ",H26,", 'name' : '",I26,"' ,'descr' : '",J26,"', 'byte1': ",K26,", 'weight1': ",L26,", 'byte2': ",M26,", 'weight2': ",N26,", 'divider': ",O26," }," ),"")</f>
@@ -2246,21 +2264,21 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="H27">
-        <f>C27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J27" t="str">
         <f>B27</f>
-        <v>Etat (marche)</v>
+        <v>Température eau retour zone 1</v>
       </c>
       <c r="Q27" t="str">
         <f>IF(G27="Oui",_xlfn.CONCAT("{ 'stream' : ",H27,", 'name' : '",I27,"' ,'descr' : '",J27,"', 'byte1': ",K27,", 'weight1': ",L27,", 'byte2': ",M27,", 'weight2': ",N27,", 'divider': ",O27," }," ),"")</f>
@@ -2269,10 +2287,25 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>79</v>
+      </c>
+      <c r="J28" t="str">
+        <f>B28</f>
+        <v>Etat (marche)</v>
+      </c>
+      <c r="Q28" t="str">
+        <f>IF(G28="Oui",_xlfn.CONCAT("{ 'stream' : ",H28,", 'name' : '",I28,"' ,'descr' : '",J28,"', 'byte1': ",K28,", 'weight1': ",L28,", 'byte2': ",M28,", 'weight2': ",N28,", 'divider': ",O28," }," ),"")</f>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -2280,7 +2313,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -2288,20 +2321,20 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2309,16 +2342,24 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
         <v>89</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q27">
-    <sortCondition ref="C2:C27"/>
-    <sortCondition ref="K2:K27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q28">
+    <sortCondition ref="C2:C28"/>
+    <sortCondition ref="K2:K28"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2327,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA0E6119-EB0F-4A94-9FD9-76ECAE32D8E2}">
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,29 +2400,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="9" t="s">
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="18"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="13"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2396,58 +2437,58 @@
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="V2" s="8" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2461,49 +2502,49 @@
       <c r="C3" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="9">
         <v>163</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="9">
         <v>12</v>
       </c>
-      <c r="I3" s="14">
-        <f>IF(H3="","",IF($V3="","",H3-$V3))</f>
+      <c r="I3" s="9">
+        <f t="shared" ref="I3:I31" si="0">IF(H3="","",IF($V3="","",H3-$V3))</f>
         <v>12</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="10">
         <v>156</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15" t="str">
-        <f>IF(L3="","",IF($V3="","",L3-$V3))</f>
-        <v/>
-      </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14" t="str">
-        <f>IF(P3="","",IF($V3="","",P3-$V3))</f>
-        <v/>
-      </c>
-      <c r="R3" s="16" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10" t="str">
+        <f t="shared" ref="M3:M8" si="1">IF(L3="","",IF($V3="","",L3-$V3))</f>
+        <v/>
+      </c>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9" t="str">
+        <f t="shared" ref="Q3:Q9" si="2">IF(P3="","",IF($V3="","",P3-$V3))</f>
+        <v/>
+      </c>
+      <c r="R3" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16" t="s">
+      <c r="T3" s="11"/>
+      <c r="U3" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="V3" s="16">
+      <c r="V3" s="11">
         <v>0</v>
       </c>
     </row>
@@ -2517,59 +2558,59 @@
       <c r="C4" t="s">
         <v>141</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="9">
         <v>163</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="9">
         <v>24</v>
       </c>
-      <c r="I4" s="14">
-        <f>IF(H4="","",IF($V4="","",H4-$V4))</f>
+      <c r="I4" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="10">
         <v>156</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="10">
         <v>24</v>
       </c>
-      <c r="M4" s="15">
-        <f>IF(L4="","",IF($V4="","",L4-$V4))</f>
+      <c r="M4" s="10">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="9">
         <v>156</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="9">
         <v>141</v>
       </c>
-      <c r="Q4" s="14">
-        <f>IF(P4="","",IF($V4="","",P4-$V4))</f>
+      <c r="Q4" s="9">
+        <f t="shared" si="2"/>
         <v>129</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="R4" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="S4" s="16" t="s">
+      <c r="S4" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16" t="s">
+      <c r="T4" s="11"/>
+      <c r="U4" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="V4" s="16">
+      <c r="V4" s="11">
         <v>12</v>
       </c>
     </row>
@@ -2583,47 +2624,47 @@
       <c r="C5" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14" t="str">
-        <f>IF(H5="","",IF($V5="","",H5-$V5))</f>
-        <v/>
-      </c>
-      <c r="J5" s="15">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J5" s="10">
         <v>156</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="10">
         <v>52</v>
       </c>
-      <c r="M5" s="15">
-        <f>IF(L5="","",IF($V5="","",L5-$V5))</f>
+      <c r="M5" s="10">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14" t="str">
-        <f>IF(P5="","",IF($V5="","",P5-$V5))</f>
-        <v/>
-      </c>
-      <c r="R5" s="16" t="s">
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R5" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="S5" s="16" t="s">
+      <c r="S5" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16" t="s">
+      <c r="T5" s="11"/>
+      <c r="U5" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="V5" s="16">
+      <c r="V5" s="11">
         <v>40</v>
       </c>
     </row>
@@ -2637,47 +2678,47 @@
       <c r="C6" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14" t="str">
-        <f>IF(H6="","",IF($V6="","",H6-$V6))</f>
-        <v/>
-      </c>
-      <c r="J6" s="15">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J6" s="10">
         <v>156</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="10">
         <v>54</v>
       </c>
-      <c r="M6" s="15">
-        <f>IF(L6="","",IF($V6="","",L6-$V6))</f>
+      <c r="M6" s="10">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14" t="str">
-        <f>IF(P6="","",IF($V6="","",P6-$V6))</f>
-        <v/>
-      </c>
-      <c r="R6" s="16" t="s">
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R6" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="S6" s="16" t="s">
+      <c r="S6" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16" t="s">
+      <c r="T6" s="11"/>
+      <c r="U6" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="V6" s="16">
+      <c r="V6" s="11">
         <v>42</v>
       </c>
     </row>
@@ -2691,51 +2732,50 @@
       <c r="C7" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="14">
+      <c r="F7" s="9">
         <v>163</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="9">
         <v>56</v>
       </c>
-      <c r="I7" s="14">
-        <f>IF(H7="","",IF($V7="","",H7-$V7))</f>
+      <c r="I7" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="10">
         <v>156</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="10">
         <v>56</v>
       </c>
-      <c r="M7" s="15">
-        <f>IF(L7="","",IF($V7="","",L7-$V7))</f>
+      <c r="M7" s="10">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14" t="str">
-        <f>IF(P7="","",IF($V7="","",P7-$V7))</f>
-        <v/>
-      </c>
-      <c r="R7" s="16" t="s">
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R7" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="S7" s="16" t="s">
+      <c r="S7" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16" t="s">
+      <c r="T7" s="11"/>
+      <c r="U7" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="V7" s="16">
+      <c r="V7" s="11">
         <v>44</v>
       </c>
     </row>
@@ -2749,112 +2789,107 @@
       <c r="C8" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
         <v>2</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="9">
         <v>163</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="9">
         <v>62</v>
       </c>
-      <c r="I8" s="14">
-        <f>IF(H8="","",IF($V8="","",H8-$V8))</f>
+      <c r="I8" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="10">
         <v>156</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="10">
         <v>62</v>
       </c>
-      <c r="M8" s="15">
-        <f>IF(L8="","",IF($V8="","",L8-$V8))</f>
+      <c r="M8" s="10">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14" t="str">
-        <f>IF(P8="","",IF($V8="","",P8-$V8))</f>
-        <v/>
-      </c>
-      <c r="R8" s="16" t="s">
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R8" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="S8" s="16" t="s">
+      <c r="S8" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16" t="s">
+      <c r="T8" s="11"/>
+      <c r="U8" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="V8" s="16">
+      <c r="V8" s="11">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>248</v>
       </c>
       <c r="C9" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="5">
-        <v>2</v>
-      </c>
-      <c r="F9" s="14">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
         <v>227</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="14">
-        <v>30</v>
-      </c>
-      <c r="I9" s="14">
-        <f>IF(H9="","",IF($V9="","",H9-$V9))</f>
+      <c r="G9" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" s="9">
         <v>12</v>
       </c>
-      <c r="J9" s="15">
-        <v>220</v>
-      </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15" t="str">
-        <f>IF(L9="","",IF(#REF!="","",L9-#REF!))</f>
-        <v/>
-      </c>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14" t="str">
-        <f>IF(P9="","",IF(#REF!="","",P9-#REF!))</f>
-        <v/>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="S9" s="16" t="s">
+      <c r="I9" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="S9" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="T9" s="16">
-        <v>18</v>
-      </c>
-      <c r="U9" s="16" t="s">
+      <c r="T9" s="11">
+        <v>0</v>
+      </c>
+      <c r="U9" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V9" s="16">
-        <v>18</v>
+      <c r="V9" s="11">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2862,70 +2897,57 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
         <v>142</v>
       </c>
-      <c r="D10">
-        <v>54.55</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="9">
         <v>227</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="14">
-        <v>54</v>
-      </c>
-      <c r="I10" s="14">
-        <f>IF(H10="","",IF($V10="","",H10-$V10))</f>
+      <c r="G10" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="9">
+        <v>30</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="10">
         <v>220</v>
       </c>
-      <c r="K10" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="L10" s="15">
-        <v>54</v>
-      </c>
-      <c r="M10" s="15">
-        <f>IF(L10="","",IF($V10="","",L10-$V10))</f>
-        <v>12</v>
-      </c>
-      <c r="N10" s="14">
-        <v>150</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="P10" s="14">
-        <v>55</v>
-      </c>
-      <c r="Q10" s="14">
-        <f>IF(P10="","",IF($V10="","",P10-$V10))</f>
-        <v>13</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="S10" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="T10" s="16">
-        <v>2</v>
-      </c>
-      <c r="U10" s="16" t="s">
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10" t="str">
+        <f>IF(L10="","",IF(#REF!="","",L10-#REF!))</f>
+        <v/>
+      </c>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9" t="str">
+        <f>IF(P10="","",IF(#REF!="","",P10-#REF!))</f>
+        <v/>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="T10" s="11">
+        <v>18</v>
+      </c>
+      <c r="U10" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V10" s="16">
-        <v>42</v>
+      <c r="V10" s="11">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2933,70 +2955,70 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>142</v>
       </c>
       <c r="D11">
-        <v>56.57</v>
-      </c>
-      <c r="E11" s="5">
+        <v>54.55</v>
+      </c>
+      <c r="E11">
         <v>2</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="9">
         <v>227</v>
       </c>
-      <c r="G11" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="14">
-        <v>56</v>
-      </c>
-      <c r="I11" s="14">
-        <f>IF(H11="","",IF($V11="","",H11-$V11))</f>
+      <c r="G11" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="9">
+        <v>54</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="10">
         <v>220</v>
       </c>
-      <c r="K11" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="L11" s="15">
-        <v>56</v>
-      </c>
-      <c r="M11" s="15">
-        <f>IF(L11="","",IF($V11="","",L11-$V11))</f>
+      <c r="K11" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="10">
+        <v>54</v>
+      </c>
+      <c r="M11" s="10">
+        <f t="shared" ref="M11:M31" si="3">IF(L11="","",IF($V11="","",L11-$V11))</f>
         <v>12</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="9">
         <v>150</v>
       </c>
-      <c r="O11" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="P11" s="14">
-        <v>57</v>
-      </c>
-      <c r="Q11" s="14">
-        <f>IF(P11="","",IF($V11="","",P11-$V11))</f>
+      <c r="O11" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="P11" s="9">
+        <v>55</v>
+      </c>
+      <c r="Q11" s="9">
+        <f t="shared" ref="Q11:Q31" si="4">IF(P11="","",IF($V11="","",P11-$V11))</f>
         <v>13</v>
       </c>
-      <c r="R11" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="S11" s="16" t="s">
+      <c r="R11" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="S11" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="T11" s="16">
-        <v>4</v>
-      </c>
-      <c r="U11" s="16" t="s">
+      <c r="T11" s="11">
+        <v>2</v>
+      </c>
+      <c r="U11" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V11" s="16">
-        <v>44</v>
+      <c r="V11" s="11">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -3004,129 +3026,138 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="14">
+      <c r="D12">
+        <v>56.57</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
         <v>227</v>
       </c>
-      <c r="G12" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="14">
-        <v>62</v>
-      </c>
-      <c r="I12" s="14">
-        <f>IF(H12="","",IF($V12="","",H12-$V12))</f>
+      <c r="G12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="9">
+        <v>56</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="10">
         <v>220</v>
       </c>
-      <c r="K12" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="L12" s="15">
-        <v>62</v>
-      </c>
-      <c r="M12" s="15">
-        <f>IF(L12="","",IF($V12="","",L12-$V12))</f>
+      <c r="K12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="L12" s="10">
+        <v>56</v>
+      </c>
+      <c r="M12" s="10">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="9">
         <v>150</v>
       </c>
-      <c r="O12" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="P12" s="14">
-        <v>81</v>
-      </c>
-      <c r="Q12" s="14">
-        <f>IF(P12="","",IF($V12="","",P12-$V12))</f>
-        <v>31</v>
-      </c>
-      <c r="R12" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="S12" s="16" t="s">
+      <c r="O12" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="P12" s="9">
+        <v>57</v>
+      </c>
+      <c r="Q12" s="9">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="S12" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="T12" s="16">
-        <v>10</v>
-      </c>
-      <c r="U12" s="16" t="s">
+      <c r="T12" s="11">
+        <v>4</v>
+      </c>
+      <c r="U12" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V12" s="16">
-        <v>50</v>
+      <c r="V12" s="11">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="5">
-        <v>2</v>
-      </c>
-      <c r="F13" s="14">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
         <v>227</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="14">
-        <v>68</v>
-      </c>
-      <c r="I13" s="14">
-        <f>IF(H13="","",IF($V13="","",H13-$V13))</f>
+      <c r="G13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="9">
+        <v>62</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="10">
         <v>220</v>
       </c>
-      <c r="K13" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="L13" s="15">
-        <v>68</v>
-      </c>
-      <c r="M13" s="15">
-        <f>IF(L13="","",IF($V13="","",L13-$V13))</f>
+      <c r="K13" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="L13" s="10">
+        <v>62</v>
+      </c>
+      <c r="M13" s="10">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14" t="str">
-        <f>IF(P13="","",IF($V13="","",P13-$V13))</f>
-        <v/>
-      </c>
-      <c r="R13" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="S13" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="T13" s="16">
-        <v>0</v>
-      </c>
-      <c r="U13" s="16" t="s">
+      <c r="N13" s="9">
+        <v>150</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="P13" s="9">
+        <v>81</v>
+      </c>
+      <c r="Q13" s="9">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="T13" s="11">
+        <v>10</v>
+      </c>
+      <c r="U13" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V13" s="16">
-        <v>56</v>
+      <c r="V13" s="11">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -3134,64 +3165,61 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>142</v>
       </c>
-      <c r="D14">
-        <v>70.709999999999994</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="9">
         <v>227</v>
       </c>
-      <c r="G14" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="14">
-        <v>70</v>
-      </c>
-      <c r="I14" s="14">
-        <f>IF(H14="","",IF($V14="","",H14-$V14))</f>
+      <c r="G14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="9">
+        <v>68</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="10">
         <v>220</v>
       </c>
-      <c r="K14" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="L14" s="15">
-        <v>70</v>
-      </c>
-      <c r="M14" s="15">
-        <f>IF(L14="","",IF($V14="","",L14-$V14))</f>
+      <c r="K14" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="L14" s="10">
+        <v>68</v>
+      </c>
+      <c r="M14" s="10">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14" t="str">
-        <f>IF(P14="","",IF($V14="","",P14-$V14))</f>
-        <v/>
-      </c>
-      <c r="R14" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="S14" s="16" t="s">
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="S14" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="T14" s="16">
-        <v>2</v>
-      </c>
-      <c r="U14" s="16" t="s">
+      <c r="T14" s="11">
+        <v>0</v>
+      </c>
+      <c r="U14" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V14" s="16">
-        <v>58</v>
+      <c r="V14" s="11">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -3199,125 +3227,122 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
         <v>142</v>
       </c>
-      <c r="E15" s="5">
+      <c r="D15">
+        <v>70.709999999999994</v>
+      </c>
+      <c r="E15">
         <v>2</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="9">
         <v>227</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14" t="str">
-        <f>IF(H15="","",IF($V15="","",H15-$V15))</f>
-        <v/>
-      </c>
-      <c r="J15" s="15">
+      <c r="G15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="9">
+        <v>70</v>
+      </c>
+      <c r="I15" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J15" s="10">
         <v>220</v>
       </c>
-      <c r="K15" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="L15" s="15">
-        <v>80</v>
-      </c>
-      <c r="M15" s="15">
-        <f>IF(L15="","",IF($V15="","",L15-$V15))</f>
+      <c r="K15" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="L15" s="10">
+        <v>70</v>
+      </c>
+      <c r="M15" s="10">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14" t="str">
-        <f>IF(P15="","",IF($V15="","",P15-$V15))</f>
-        <v/>
-      </c>
-      <c r="R15" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="S15" s="16" t="s">
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="S15" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="T15" s="16">
-        <v>14</v>
-      </c>
-      <c r="U15" s="16" t="s">
+      <c r="T15" s="11">
+        <v>2</v>
+      </c>
+      <c r="U15" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V15" s="16">
-        <v>68</v>
+      <c r="V15" s="11">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="C16" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16">
         <v>2</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="9">
         <v>227</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J16" s="10">
+        <v>220</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="L16" s="10">
         <v>80</v>
       </c>
-      <c r="H16" s="14">
-        <v>108</v>
-      </c>
-      <c r="I16" s="14">
-        <f>IF(H16="","",IF($V16="","",H16-$V16))</f>
+      <c r="M16" s="10">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="J16" s="15">
-        <v>220</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L16" s="15">
-        <v>108</v>
-      </c>
-      <c r="M16" s="15">
-        <f>IF(L16="","",IF($V16="","",L16-$V16))</f>
-        <v>12</v>
-      </c>
-      <c r="N16" s="14">
-        <v>150</v>
-      </c>
-      <c r="O16" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="P16" s="14">
-        <v>71</v>
-      </c>
-      <c r="Q16" s="14">
-        <f>IF(P16="","",IF($V16="","",P16-$V16))</f>
-        <v>-25</v>
-      </c>
-      <c r="R16" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="S16" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="T16" s="16">
-        <v>0</v>
-      </c>
-      <c r="U16" s="16" t="s">
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="T16" s="11">
+        <v>14</v>
+      </c>
+      <c r="U16" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V16" s="16">
-        <v>96</v>
+      <c r="V16" s="11">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -3325,669 +3350,723 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
         <v>142</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17">
         <v>2</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="9">
         <v>227</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="H17" s="14">
-        <v>110</v>
-      </c>
-      <c r="I17" s="14">
-        <f>IF(H17="","",IF($V17="","",H17-$V17))</f>
+      <c r="G17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="9">
+        <v>108</v>
+      </c>
+      <c r="I17" s="9">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="10">
         <v>220</v>
       </c>
-      <c r="K17" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="L17" s="15">
-        <v>110</v>
-      </c>
-      <c r="M17" s="15">
-        <f>IF(L17="","",IF($V17="","",L17-$V17))</f>
+      <c r="K17" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="L17" s="10">
+        <v>108</v>
+      </c>
+      <c r="M17" s="10">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17" s="9">
         <v>150</v>
       </c>
-      <c r="O17" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="P17" s="14">
-        <v>73</v>
-      </c>
-      <c r="Q17" s="14">
-        <f>IF(P17="","",IF($V17="","",P17-$V17))</f>
+      <c r="O17" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="P17" s="9">
+        <v>71</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" si="4"/>
         <v>-25</v>
       </c>
-      <c r="R17" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="S17" s="16" t="s">
+      <c r="R17" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="S17" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="T17" s="16">
-        <v>2</v>
-      </c>
-      <c r="U17" s="16" t="s">
+      <c r="T17" s="11">
+        <v>0</v>
+      </c>
+      <c r="U17" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V17" s="16">
-        <v>98</v>
+      <c r="V17" s="11">
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="14">
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="9">
         <v>227</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14" t="str">
-        <f>IF(H18="","",IF($V18="","",H18-$V18))</f>
-        <v/>
-      </c>
-      <c r="J18" s="15">
+      <c r="G18" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="9">
+        <v>110</v>
+      </c>
+      <c r="I18" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J18" s="10">
         <v>220</v>
       </c>
-      <c r="K18" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="L18" s="15">
-        <v>178</v>
-      </c>
-      <c r="M18" s="15" t="str">
-        <f>IF(L18="","",IF($V18="","",L18-$V18))</f>
-        <v/>
-      </c>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14" t="str">
-        <f>IF(P18="","",IF($V18="","",P18-$V18))</f>
-        <v/>
-      </c>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
+      <c r="K18" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L18" s="10">
+        <v>110</v>
+      </c>
+      <c r="M18" s="10">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="N18" s="9">
+        <v>150</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="P18" s="9">
+        <v>73</v>
+      </c>
+      <c r="Q18" s="9">
+        <f t="shared" si="4"/>
+        <v>-25</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="T18" s="11">
+        <v>2</v>
+      </c>
+      <c r="U18" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="V18" s="11">
+        <v>98</v>
+      </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s">
         <v>142</v>
       </c>
-      <c r="D19">
-        <v>168</v>
-      </c>
-      <c r="F19" s="14">
+      <c r="F19" s="9">
         <v>227</v>
       </c>
-      <c r="G19" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="14">
-        <v>168</v>
-      </c>
-      <c r="I19" s="14" t="str">
-        <f>IF(H19="","",IF($V19="","",H19-$V19))</f>
-        <v/>
-      </c>
-      <c r="J19" s="15">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J19" s="10">
         <v>220</v>
       </c>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15" t="str">
-        <f>IF(L19="","",IF($V19="","",L19-$V19))</f>
-        <v/>
-      </c>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14" t="str">
-        <f>IF(P19="","",IF($V19="","",P19-$V19))</f>
-        <v/>
-      </c>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
+      <c r="K19" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L19" s="10">
+        <v>178</v>
+      </c>
+      <c r="M19" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>142</v>
       </c>
       <c r="D20">
-        <v>169</v>
-      </c>
-      <c r="F20" s="14">
+        <v>168</v>
+      </c>
+      <c r="F20" s="9">
         <v>227</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="14">
-        <v>169</v>
-      </c>
-      <c r="I20" s="14" t="str">
-        <f>IF(H20="","",IF($V20="","",H20-$V20))</f>
-        <v/>
-      </c>
-      <c r="J20" s="15">
+      <c r="H20" s="9">
+        <v>168</v>
+      </c>
+      <c r="I20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J20" s="10">
         <v>220</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15" t="str">
-        <f>IF(L20="","",IF($V20="","",L20-$V20))</f>
-        <v/>
-      </c>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14" t="str">
-        <f>IF(P20="","",IF($V20="","",P20-$V20))</f>
-        <v/>
-      </c>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>142</v>
       </c>
       <c r="D21">
-        <v>170</v>
-      </c>
-      <c r="F21" s="14">
+        <v>169</v>
+      </c>
+      <c r="F21" s="9">
         <v>227</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="14">
-        <v>170</v>
-      </c>
-      <c r="I21" s="14" t="str">
-        <f>IF(H21="","",IF($V21="","",H21-$V21))</f>
-        <v/>
-      </c>
-      <c r="J21" s="15">
+      <c r="H21" s="9">
+        <v>169</v>
+      </c>
+      <c r="I21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J21" s="10">
         <v>220</v>
       </c>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15" t="str">
-        <f>IF(L21="","",IF($V21="","",L21-$V21))</f>
-        <v/>
-      </c>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14" t="str">
-        <f>IF(P21="","",IF($V21="","",P21-$V21))</f>
-        <v/>
-      </c>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
         <v>142</v>
       </c>
       <c r="D22">
-        <v>171</v>
-      </c>
-      <c r="F22" s="14">
+        <v>170</v>
+      </c>
+      <c r="F22" s="9">
         <v>227</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="14">
-        <v>171</v>
-      </c>
-      <c r="I22" s="14" t="str">
-        <f>IF(H22="","",IF($V22="","",H22-$V22))</f>
-        <v/>
-      </c>
-      <c r="J22" s="15">
+      <c r="H22" s="9">
+        <v>170</v>
+      </c>
+      <c r="I22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J22" s="10">
         <v>220</v>
       </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15" t="str">
-        <f>IF(L22="","",IF($V22="","",L22-$V22))</f>
-        <v/>
-      </c>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14" t="str">
-        <f>IF(P22="","",IF($V22="","",P22-$V22))</f>
-        <v/>
-      </c>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>142</v>
       </c>
       <c r="D23">
-        <v>172</v>
-      </c>
-      <c r="F23" s="14">
+        <v>171</v>
+      </c>
+      <c r="F23" s="9">
         <v>227</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="14">
-        <v>172</v>
-      </c>
-      <c r="I23" s="14" t="str">
-        <f>IF(H23="","",IF($V23="","",H23-$V23))</f>
-        <v/>
-      </c>
-      <c r="J23" s="15">
+      <c r="H23" s="9">
+        <v>171</v>
+      </c>
+      <c r="I23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J23" s="10">
         <v>220</v>
       </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15" t="str">
-        <f>IF(L23="","",IF($V23="","",L23-$V23))</f>
-        <v/>
-      </c>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14" t="str">
-        <f>IF(P23="","",IF($V23="","",P23-$V23))</f>
-        <v/>
-      </c>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
         <v>142</v>
       </c>
       <c r="D24">
-        <v>173</v>
-      </c>
-      <c r="F24" s="14">
+        <v>172</v>
+      </c>
+      <c r="F24" s="9">
         <v>227</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="14">
-        <v>173</v>
-      </c>
-      <c r="I24" s="14" t="str">
-        <f>IF(H24="","",IF($V24="","",H24-$V24))</f>
-        <v/>
-      </c>
-      <c r="J24" s="15">
+      <c r="H24" s="9">
+        <v>172</v>
+      </c>
+      <c r="I24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J24" s="10">
         <v>220</v>
       </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15" t="str">
-        <f>IF(L24="","",IF($V24="","",L24-$V24))</f>
-        <v/>
-      </c>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14" t="str">
-        <f>IF(P24="","",IF($V24="","",P24-$V24))</f>
-        <v/>
-      </c>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>142</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="14">
+      <c r="D25">
+        <v>173</v>
+      </c>
+      <c r="F25" s="9">
         <v>227</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14" t="str">
-        <f>IF(H25="","",IF($V25="","",H25-$V25))</f>
-        <v/>
-      </c>
-      <c r="J25" s="15">
+      <c r="G25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="9">
+        <v>173</v>
+      </c>
+      <c r="I25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J25" s="10">
         <v>220</v>
       </c>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15" t="str">
-        <f>IF(L25="","",IF($V25="","",L25-$V25))</f>
-        <v/>
-      </c>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14" t="str">
-        <f>IF(P25="","",IF($V25="","",P25-$V25))</f>
-        <v/>
-      </c>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-      <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="14">
+      <c r="F26" s="9">
         <v>227</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="H26" s="14">
-        <v>193</v>
-      </c>
-      <c r="I26" s="14" t="str">
-        <f>IF(H26="","",IF($V26="","",H26-$V26))</f>
-        <v/>
-      </c>
-      <c r="J26" s="15">
+      <c r="G26" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J26" s="10">
         <v>220</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="L26" s="15">
-        <v>193</v>
-      </c>
-      <c r="M26" s="15" t="str">
-        <f>IF(L26="","",IF($V26="","",L26-$V26))</f>
-        <v/>
-      </c>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14" t="str">
-        <f>IF(P26="","",IF($V26="","",P26-$V26))</f>
-        <v/>
-      </c>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="14">
-        <v>0</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="14">
-        <v>0</v>
-      </c>
-      <c r="I27" s="14" t="str">
-        <f>IF(H27="","",IF($V27="","",H27-$V27))</f>
-        <v/>
-      </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15" t="str">
-        <f>IF(L27="","",IF($V27="","",L27-$V27))</f>
-        <v/>
-      </c>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14" t="str">
-        <f>IF(P27="","",IF($V27="","",P27-$V27))</f>
-        <v/>
-      </c>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
+        <v>143</v>
+      </c>
+      <c r="C27" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="9">
+        <v>227</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" s="9">
+        <v>193</v>
+      </c>
+      <c r="I27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J27" s="10">
+        <v>220</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="L27" s="10">
+        <v>193</v>
+      </c>
+      <c r="M27" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="14">
-        <v>0</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14" t="str">
-        <f>IF(H28="","",IF($V28="","",H28-$V28))</f>
-        <v/>
-      </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15" t="str">
-        <f>IF(L28="","",IF($V28="","",L28-$V28))</f>
-        <v/>
-      </c>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14" t="str">
-        <f>IF(P28="","",IF($V28="","",P28-$V28))</f>
-        <v/>
-      </c>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0</v>
+      </c>
+      <c r="I28" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="14">
-        <v>0</v>
-      </c>
-      <c r="G29" s="14" t="s">
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14" t="str">
-        <f>IF(H29="","",IF($V29="","",H29-$V29))</f>
-        <v/>
-      </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15" t="str">
-        <f>IF(L29="","",IF($V29="","",L29-$V29))</f>
-        <v/>
-      </c>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14" t="str">
-        <f>IF(P29="","",IF($V29="","",P29-$V29))</f>
-        <v/>
-      </c>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-    </row>
-    <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="H30" s="9"/>
+      <c r="I30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+    </row>
+    <row r="31" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="14">
-        <v>0</v>
-      </c>
-      <c r="G30" s="14" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14" t="str">
-        <f>IF(H30="","",IF($V30="","",H30-$V30))</f>
-        <v/>
-      </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15" t="str">
-        <f>IF(L30="","",IF($V30="","",L30-$V30))</f>
-        <v/>
-      </c>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14" t="str">
-        <f>IF(P30="","",IF($V30="","",P30-$V30))</f>
-        <v/>
-      </c>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" t="s">
-        <v>82</v>
-      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3995,20 +4074,20 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4016,9 +4095,17 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
         <v>89</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4034,10 +4121,368 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD88252-2FFB-4A22-BE3E-7F0023A640E3}">
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="7" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>211</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>210</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>212</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>213</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>214</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>215</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>216</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>217</v>
+      </c>
+      <c r="H16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>221</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>222</v>
+      </c>
+      <c r="H21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>223</v>
+      </c>
+      <c r="H22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>226</v>
+      </c>
+      <c r="H24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>227</v>
+      </c>
+      <c r="H25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>228</v>
+      </c>
+      <c r="H26">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>229</v>
+      </c>
+      <c r="H27">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>230</v>
+      </c>
+      <c r="H28">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>231</v>
+      </c>
+      <c r="H29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>232</v>
+      </c>
+      <c r="H30">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>233</v>
+      </c>
+      <c r="H31">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>234</v>
+      </c>
+      <c r="H32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>236</v>
+      </c>
+      <c r="B33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>243</v>
+      </c>
+      <c r="H34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>244</v>
+      </c>
+      <c r="H35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>240</v>
+      </c>
+      <c r="H37">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>237</v>
+      </c>
+      <c r="B39">
+        <v>16</v>
+      </c>
+      <c r="H39">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>238</v>
+      </c>
+      <c r="H40">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>239</v>
+      </c>
+      <c r="H41">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>240</v>
+      </c>
+      <c r="H42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>241</v>
+      </c>
+      <c r="H44">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3538B6EB-3CC8-4E96-94B3-632A11E7521D}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4498,364 +4943,6 @@
       </c>
       <c r="I41">
         <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD88252-2FFB-4A22-BE3E-7F0023A640E3}">
-  <dimension ref="A1:H44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39:H41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" customWidth="1"/>
-    <col min="5" max="7" width="6.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>204</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>205</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>206</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>207</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>211</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>209</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>212</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>213</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>214</v>
-      </c>
-      <c r="H13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>215</v>
-      </c>
-      <c r="H14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>216</v>
-      </c>
-      <c r="H15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>217</v>
-      </c>
-      <c r="H16">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>221</v>
-      </c>
-      <c r="H20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>222</v>
-      </c>
-      <c r="H21">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>223</v>
-      </c>
-      <c r="H22">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>224</v>
-      </c>
-      <c r="B23">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>226</v>
-      </c>
-      <c r="H24">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>227</v>
-      </c>
-      <c r="H25">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>228</v>
-      </c>
-      <c r="H26">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>229</v>
-      </c>
-      <c r="H27">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>230</v>
-      </c>
-      <c r="H28">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>231</v>
-      </c>
-      <c r="H29">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>232</v>
-      </c>
-      <c r="H30">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>233</v>
-      </c>
-      <c r="H31">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>234</v>
-      </c>
-      <c r="H32">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>236</v>
-      </c>
-      <c r="B33">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>243</v>
-      </c>
-      <c r="H34">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>244</v>
-      </c>
-      <c r="H35">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>240</v>
-      </c>
-      <c r="H37">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>237</v>
-      </c>
-      <c r="B39">
-        <v>16</v>
-      </c>
-      <c r="H39">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>238</v>
-      </c>
-      <c r="H40">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>239</v>
-      </c>
-      <c r="H41">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>240</v>
-      </c>
-      <c r="H42">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>241</v>
-      </c>
-      <c r="H44">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Typos and new values (thx @astrotophe03 )
</commit_message>
<xml_diff>
--- a/decoder.xlsx
+++ b/decoder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\arkteos_reg3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E073F68-4BC1-42AE-9106-4C15B660FFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F779D58E-0CD3-4A8B-BBD1-D4729B686E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="32220" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="294">
   <si>
     <t>Donnée</t>
   </si>
@@ -366,9 +366,6 @@
     <t>Voltage DC groupe frigo 1</t>
   </si>
   <si>
-    <t>Vitesse ventalisateur groupe frigo 1</t>
-  </si>
-  <si>
     <t>active_error_reg</t>
   </si>
   <si>
@@ -859,6 +856,75 @@
   </si>
   <si>
     <t>[46]</t>
+  </si>
+  <si>
+    <t>Vitesse ventilateur groupe frigo 1</t>
+  </si>
+  <si>
+    <t>Puissance instantanée produite</t>
+  </si>
+  <si>
+    <t>Puissance instantanée consommée</t>
+  </si>
+  <si>
+    <t>([52]+[53]*256)/10</t>
+  </si>
+  <si>
+    <t>primaire_temp_eau_consigne</t>
+  </si>
+  <si>
+    <t>Débit eau primaire</t>
+  </si>
+  <si>
+    <t>([60]+[61]*256)/10</t>
+  </si>
+  <si>
+    <t>primaire_debit_eau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consigne température eau primaire </t>
+  </si>
+  <si>
+    <t>Consigne % circulateur primaire</t>
+  </si>
+  <si>
+    <t>[64]</t>
+  </si>
+  <si>
+    <t>primaire_circulateur_consigne</t>
+  </si>
+  <si>
+    <t>([147]+[148]*256)</t>
+  </si>
+  <si>
+    <t>nb_cycles_compresseur</t>
+  </si>
+  <si>
+    <t>Temps mise sous tension PAC</t>
+  </si>
+  <si>
+    <t>Temps de fonctionnement compresseur</t>
+  </si>
+  <si>
+    <t>Temps de fonctionnement PAC</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Nombre de cycles compresseur ? Geotwin ?</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>([42]+[43]*256)*100</t>
+  </si>
+  <si>
+    <t>Nombre de cycles compresseur (arrondi à 100)</t>
+  </si>
+  <si>
+    <t>0.01</t>
   </si>
 </sst>
 </file>
@@ -974,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1003,6 +1069,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1284,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1299,6 +1368,7 @@
     <col min="8" max="8" width="6.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="2"/>
     <col min="17" max="17" width="145.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1342,11 +1412,11 @@
       <c r="N1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="17" t="s">
         <v>52</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>87</v>
@@ -1357,22 +1427,22 @@
         <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2">
         <v>163</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H2">
         <v>163</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K2">
         <v>12</v>
@@ -1386,11 +1456,11 @@
       <c r="N2">
         <v>256</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="2">
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
@@ -1432,11 +1502,11 @@
       <c r="N3">
         <v>256</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="2">
         <v>10</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q26" si="0">IF(G3="Oui",_xlfn.CONCAT("{ 'stream' : ",H3,", 'name' : '",I3,"' ,'descr' : '",J3,"', 'byte1': ",K3,", 'weight1': ",L3,", 'byte2': ",M3,", 'weight2': ",N3,", 'divider': ",O3," }," ),"")</f>
+        <f t="shared" ref="Q3:Q31" si="0">IF(G3="Oui",_xlfn.CONCAT("{ 'stream' : ",H3,", 'name' : '",I3,"' ,'descr' : '",J3,"', 'byte1': ",K3,", 'weight1': ",L3,", 'byte2': ",M3,", 'weight2': ",N3,", 'divider': ",O3," }," ),"")</f>
         <v>{ 'stream' : 163, 'name' : 'exterieur_temp' ,'descr' : 'Température extérieure', 'byte1': 24, 'weight1': 1, 'byte2': 25, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
@@ -1444,12 +1514,15 @@
       <c r="A4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>137</v>
+      <c r="B4" t="s">
+        <v>292</v>
       </c>
       <c r="C4">
         <v>163</v>
       </c>
+      <c r="D4" t="s">
+        <v>291</v>
+      </c>
       <c r="G4" t="s">
         <v>68</v>
       </c>
@@ -1457,29 +1530,30 @@
         <v>163</v>
       </c>
       <c r="I4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" t="s">
-        <v>137</v>
+        <v>284</v>
+      </c>
+      <c r="J4" t="str">
+        <f>B4</f>
+        <v>Nombre de cycles compresseur (arrondi à 100)</v>
       </c>
       <c r="K4">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
       <c r="M4">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="N4">
         <v>256</v>
       </c>
-      <c r="O4">
-        <v>1</v>
+      <c r="O4" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="0"/>
-        <v>{ 'stream' : 163, 'name' : 'freq_comp_actuelle' ,'descr' : 'Fréquence compresseur actuelle', 'byte1': 52, 'weight1': 1, 'byte2': 53, 'weight2': 256, 'divider': 1 },</v>
+        <v>{ 'stream' : 163, 'name' : 'nb_cycles_compresseur' ,'descr' : 'Nombre de cycles compresseur (arrondi à 100)', 'byte1': 42, 'weight1': 1, 'byte2': 43, 'weight2': 256, 'divider': 0.01 },</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -1487,7 +1561,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5">
         <v>163</v>
@@ -1499,37 +1573,37 @@
         <v>163</v>
       </c>
       <c r="I5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K5">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
       <c r="M5">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N5">
         <v>256</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="2">
         <v>1</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
-        <v>{ 'stream' : 163, 'name' : 'freq_comp_cible' ,'descr' : 'Fréquence compresseur cible', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 1 },</v>
+        <v>{ 'stream' : 163, 'name' : 'freq_comp_actuelle' ,'descr' : 'Fréquence compresseur actuelle', 'byte1': 52, 'weight1': 1, 'byte2': 53, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>103</v>
       </c>
-      <c r="B6" t="s">
-        <v>86</v>
+      <c r="B6" s="15" t="s">
+        <v>137</v>
       </c>
       <c r="C6">
         <v>163</v>
@@ -1541,29 +1615,29 @@
         <v>163</v>
       </c>
       <c r="I6" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="J6" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="K6">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="M6">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N6">
         <v>256</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="2">
         <v>1</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
-        <v>{ 'stream' : 163, 'name' : 'fan_speed_evaporator_1' ,'descr' : 'Vitesse ventalisateur groupe frigo 1', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 1 },</v>
+        <v>{ 'stream' : 163, 'name' : 'freq_comp_cible' ,'descr' : 'Fréquence compresseur cible', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
@@ -1571,7 +1645,7 @@
         <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C7">
         <v>163</v>
@@ -1583,121 +1657,121 @@
         <v>163</v>
       </c>
       <c r="I7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J7" t="s">
-        <v>106</v>
+        <v>271</v>
       </c>
       <c r="K7">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="M7">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="N7">
         <v>256</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="2">
         <v>1</v>
       </c>
       <c r="Q7" t="str">
-        <f>IF(G7="Oui",_xlfn.CONCAT("{ 'stream' : ",H7,", 'name' : '",I7,"' ,'descr' : '",J7,"', 'byte1': ",K7,", 'weight1': ",L7,", 'byte2': ",M7,", 'weight2': ",N7,", 'divider': ",O7," }," ),"")</f>
-        <v>{ 'stream' : 163, 'name' : 'dc_voltage' ,'descr' : 'Voltage DC groupe frigo 1', 'byte1': 62, 'weight1': 1, 'byte2': 63, 'weight2': 256, 'divider': 1 },</v>
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 163, 'name' : 'fan_speed_evaporator_1' ,'descr' : 'Vitesse ventilateur groupe frigo 1', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>247</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>104</v>
       </c>
       <c r="C8">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="G8" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="H8">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="I8" t="s">
-        <v>249</v>
+        <v>105</v>
       </c>
       <c r="J8" t="s">
-        <v>248</v>
+        <v>106</v>
       </c>
       <c r="K8">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
+        <v>256</v>
+      </c>
+      <c r="O8" s="2">
         <v>1</v>
       </c>
       <c r="Q8" t="str">
         <f>IF(G8="Oui",_xlfn.CONCAT("{ 'stream' : ",H8,", 'name' : '",I8,"' ,'descr' : '",J8,"', 'byte1': ",K8,", 'weight1': ",L8,", 'byte2': ",M8,", 'weight2': ",N8,", 'divider': ",O8," }," ),"")</f>
-        <v/>
+        <v>{ 'stream' : 163, 'name' : 'dc_voltage' ,'descr' : 'Voltage DC groupe frigo 1', 'byte1': 62, 'weight1': 1, 'byte2': 63, 'weight2': 256, 'divider': 1 },</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" t="s">
         <v>247</v>
       </c>
-      <c r="B9" t="s">
-        <v>253</v>
-      </c>
       <c r="C9">
         <v>227</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="H9">
         <v>227</v>
       </c>
       <c r="I9" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="J9" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="K9">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>256</v>
-      </c>
-      <c r="O9">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1</v>
       </c>
       <c r="Q9" t="str">
         <f>IF(G9="Oui",_xlfn.CONCAT("{ 'stream' : ",H9,", 'name' : '",I9,"' ,'descr' : '",J9,"', 'byte1': ",K9,", 'weight1': ",L9,", 'byte2': ",M9,", 'weight2': ",N9,", 'divider': ",O9," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'puissance_inst_produite' ,'descr' : 'Puissance instanée produite', 'byte1': 16, 'weight1': 1, 'byte2': 17, 'weight2': 256, 'divider': 0,1 },</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B10" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="C10">
         <v>227</v>
@@ -1709,622 +1783,675 @@
         <v>227</v>
       </c>
       <c r="I10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J10" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="K10">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N10">
         <v>256</v>
       </c>
-      <c r="O10">
-        <v>0.1</v>
+      <c r="O10" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="Q10" t="str">
         <f>IF(G10="Oui",_xlfn.CONCAT("{ 'stream' : ",H10,", 'name' : '",I10,"' ,'descr' : '",J10,"', 'byte1': ",K10,", 'weight1': ",L10,", 'byte2': ",M10,", 'weight2': ",N10,", 'divider': ",O10," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'puissance_inst_consommee' ,'descr' : 'Puissance instanée consommée', 'byte1': 18, 'weight1': 1, 'byte2': 19, 'weight2': 256, 'divider': 0,1 },</v>
+        <v>{ 'stream' : 227, 'name' : 'puissance_inst_produite' ,'descr' : 'Puissance instantanée produite', 'byte1': 16, 'weight1': 1, 'byte2': 17, 'weight2': 256, 'divider': 0.1 },</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>273</v>
       </c>
       <c r="C11">
         <v>227</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="H11">
         <v>227</v>
       </c>
       <c r="I11" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="J11" t="s">
-        <v>113</v>
+        <v>273</v>
       </c>
       <c r="K11">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="N11">
         <v>256</v>
       </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11" t="s">
-        <v>114</v>
+      <c r="O11" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="Q11" t="str">
         <f>IF(G11="Oui",_xlfn.CONCAT("{ 'stream' : ",H11,", 'name' : '",I11,"' ,'descr' : '",J11,"', 'byte1': ",K11,", 'weight1': ",L11,", 'byte2': ",M11,", 'weight2': ",N11,", 'divider': ",O11," }," ),"")</f>
-        <v/>
+        <v>{ 'stream' : 227, 'name' : 'puissance_inst_consommee' ,'descr' : 'Puissance instantanée consommée', 'byte1': 18, 'weight1': 1, 'byte2': 19, 'weight2': 256, 'divider': 0.1 },</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B12" t="s">
-        <v>269</v>
+        <v>108</v>
       </c>
       <c r="C12">
         <v>227</v>
       </c>
-      <c r="D12" t="s">
-        <v>271</v>
-      </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="H12">
         <v>227</v>
       </c>
       <c r="I12" t="s">
-        <v>270</v>
+        <v>107</v>
       </c>
       <c r="J12" t="s">
-        <v>269</v>
+        <v>112</v>
       </c>
       <c r="K12">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
+        <v>256</v>
+      </c>
+      <c r="O12" s="2">
         <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>113</v>
       </c>
       <c r="Q12" t="str">
         <f>IF(G12="Oui",_xlfn.CONCAT("{ 'stream' : ",H12,", 'name' : '",I12,"' ,'descr' : '",J12,"', 'byte1': ",K12,", 'weight1': ",L12,", 'byte2': ",M12,", 'weight2': ",N12,", 'divider': ",O12," }," ),"")</f>
-        <v>{ 'stream' : 227, 'name' : 'modele_pac' ,'descr' : 'Modèle PAC', 'byte1': 46, 'weight1': 1, 'byte2': 0, 'weight2': 0, 'divider': 1 },</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>268</v>
       </c>
       <c r="C13">
         <v>227</v>
       </c>
-      <c r="E13">
-        <v>54.55</v>
+      <c r="D13" t="s">
+        <v>270</v>
       </c>
       <c r="G13" t="s">
         <v>68</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:H32" si="1">C13</f>
         <v>227</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" ref="J13:J26" si="2">B13</f>
-        <v>Température eau primaire aller</v>
+        <v>269</v>
+      </c>
+      <c r="J13" t="s">
+        <v>268</v>
       </c>
       <c r="K13">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
       <c r="M13">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>256</v>
-      </c>
-      <c r="O13">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="0"/>
-        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_aller' ,'descr' : 'Température eau primaire aller', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 10 },</v>
+        <f>IF(G13="Oui",_xlfn.CONCAT("{ 'stream' : ",H13,", 'name' : '",I13,"' ,'descr' : '",J13,"', 'byte1': ",K13,", 'weight1': ",L13,", 'byte2': ",M13,", 'weight2': ",N13,", 'divider': ",O13," }," ),"")</f>
+        <v>{ 'stream' : 227, 'name' : 'modele_pac' ,'descr' : 'Modèle PAC', 'byte1': 46, 'weight1': 1, 'byte2': 0, 'weight2': 0, 'divider': 1 },</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>276</v>
       </c>
       <c r="C14">
         <v>227</v>
       </c>
-      <c r="E14">
-        <v>56.57</v>
+      <c r="D14" t="s">
+        <v>277</v>
       </c>
       <c r="G14" t="s">
         <v>68</v>
       </c>
       <c r="H14">
+        <v>227</v>
+      </c>
+      <c r="I14" t="s">
+        <v>278</v>
+      </c>
+      <c r="J14" t="str">
+        <f>B14</f>
+        <v>Débit eau primaire</v>
+      </c>
+      <c r="K14">
+        <v>60</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>61</v>
+      </c>
+      <c r="N14">
+        <v>256</v>
+      </c>
+      <c r="O14" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q14" t="str">
+        <f>IF(G14="Oui",_xlfn.CONCAT("{ 'stream' : ",H14,", 'name' : '",I14,"' ,'descr' : '",J14,"', 'byte1': ",K14,", 'weight1': ",L14,", 'byte2': ",M14,", 'weight2': ",N14,", 'divider': ",O14," }," ),"")</f>
+        <v>{ 'stream' : 227, 'name' : 'primaire_debit_eau' ,'descr' : 'Débit eau primaire', 'byte1': 60, 'weight1': 1, 'byte2': 61, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" t="s">
+        <v>279</v>
+      </c>
+      <c r="C15">
+        <v>227</v>
+      </c>
+      <c r="D15" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15">
+        <v>227</v>
+      </c>
+      <c r="I15" t="s">
+        <v>275</v>
+      </c>
+      <c r="J15" t="str">
+        <f>B15</f>
+        <v xml:space="preserve">Consigne température eau primaire </v>
+      </c>
+      <c r="K15">
+        <v>52</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>53</v>
+      </c>
+      <c r="N15">
+        <v>256</v>
+      </c>
+      <c r="O15" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q15" t="str">
+        <f>IF(G15="Oui",_xlfn.CONCAT("{ 'stream' : ",H15,", 'name' : '",I15,"' ,'descr' : '",J15,"', 'byte1': ",K15,", 'weight1': ",L15,", 'byte2': ",M15,", 'weight2': ",N15,", 'divider': ",O15," }," ),"")</f>
+        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_consigne' ,'descr' : 'Consigne température eau primaire ', 'byte1': 52, 'weight1': 1, 'byte2': 53, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>227</v>
+      </c>
+      <c r="E16">
+        <v>54.55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H37" si="1">C16</f>
+        <v>227</v>
+      </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" ref="J16:J31" si="2">B16</f>
+        <v>Température eau primaire aller</v>
+      </c>
+      <c r="K16">
+        <v>54</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>55</v>
+      </c>
+      <c r="N16">
+        <v>256</v>
+      </c>
+      <c r="O16" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_aller' ,'descr' : 'Température eau primaire aller', 'byte1': 54, 'weight1': 1, 'byte2': 55, 'weight2': 256, 'divider': 10 },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>227</v>
+      </c>
+      <c r="E17">
+        <v>56.57</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I17" t="s">
         <v>72</v>
       </c>
-      <c r="J14" t="str">
+      <c r="J17" t="str">
         <f t="shared" si="2"/>
         <v>Température eau primaire retour</v>
       </c>
-      <c r="K14">
+      <c r="K17">
         <v>56</v>
       </c>
-      <c r="L14">
+      <c r="L17">
         <v>1</v>
       </c>
-      <c r="M14">
+      <c r="M17">
         <v>57</v>
       </c>
-      <c r="N14">
+      <c r="N17">
         <v>256</v>
       </c>
-      <c r="O14">
+      <c r="O17" s="2">
         <v>10</v>
       </c>
-      <c r="Q14" t="str">
+      <c r="Q17" t="str">
         <f t="shared" si="0"/>
         <v>{ 'stream' : 227, 'name' : 'primaire_temp_eau_retour' ,'descr' : 'Température eau primaire retour', 'byte1': 56, 'weight1': 1, 'byte2': 57, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>247</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" t="s">
         <v>67</v>
       </c>
-      <c r="C15">
-        <v>227</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C18">
+        <v>227</v>
+      </c>
+      <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G18" t="s">
         <v>68</v>
       </c>
-      <c r="H15">
+      <c r="H18">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I18" t="s">
         <v>70</v>
       </c>
-      <c r="J15" t="str">
+      <c r="J18" t="str">
         <f t="shared" si="2"/>
         <v>Pression eau primaire</v>
       </c>
-      <c r="K15">
+      <c r="K18">
         <v>62</v>
       </c>
-      <c r="L15">
+      <c r="L18">
         <v>1</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
         <v>10</v>
       </c>
-      <c r="Q15" t="str">
+      <c r="Q18" t="str">
         <f t="shared" si="0"/>
         <v>{ 'stream' : 227, 'name' : 'primaire_pression' ,'descr' : 'Pression eau primaire', 'byte1': 62, 'weight1': 1, 'byte2': 0, 'weight2': 0, 'divider': 10 },</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
+        <v>280</v>
+      </c>
+      <c r="C19">
+        <v>227</v>
+      </c>
+      <c r="D19" t="s">
+        <v>281</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19">
+        <f>C19</f>
+        <v>227</v>
+      </c>
+      <c r="I19" t="s">
+        <v>282</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="2"/>
+        <v>Consigne % circulateur primaire</v>
+      </c>
+      <c r="K19">
+        <v>64</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'stream' : 227, 'name' : 'primaire_circulateur_consigne' ,'descr' : 'Consigne % circulateur primaire', 'byte1': 64, 'weight1': 1, 'byte2': 0, 'weight2': 0, 'divider': 1 },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
         <v>46</v>
       </c>
-      <c r="C16">
-        <v>227</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C20">
+        <v>227</v>
+      </c>
+      <c r="D20" t="s">
         <v>26</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G20" t="s">
         <v>68</v>
       </c>
-      <c r="H16">
+      <c r="H20">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I20" t="s">
         <v>75</v>
       </c>
-      <c r="J16" t="str">
+      <c r="J20" t="str">
         <f t="shared" si="2"/>
         <v>Température intérieur zone 1</v>
       </c>
-      <c r="K16">
+      <c r="K20">
         <v>68</v>
       </c>
-      <c r="L16">
+      <c r="L20">
         <v>1</v>
       </c>
-      <c r="M16">
+      <c r="M20">
         <v>69</v>
       </c>
-      <c r="N16">
+      <c r="N20">
         <v>256</v>
       </c>
-      <c r="O16">
+      <c r="O20" s="2">
         <v>10</v>
       </c>
-      <c r="Q16" t="str">
+      <c r="Q20" t="str">
         <f t="shared" si="0"/>
         <v>{ 'stream' : 227, 'name' : 'zone1_temp_interieur' ,'descr' : 'Température intérieur zone 1', 'byte1': 68, 'weight1': 1, 'byte2': 69, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" t="s">
         <v>35</v>
       </c>
-      <c r="C17">
-        <v>227</v>
-      </c>
-      <c r="E17">
+      <c r="C21">
+        <v>227</v>
+      </c>
+      <c r="E21">
         <v>70.709999999999994</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G21" t="s">
         <v>68</v>
       </c>
-      <c r="H17">
+      <c r="H21">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I21" t="s">
         <v>78</v>
       </c>
-      <c r="J17" t="str">
+      <c r="J21" t="str">
         <f t="shared" si="2"/>
         <v>Consigne intérieure zone 1</v>
       </c>
-      <c r="K17">
+      <c r="K21">
         <v>70</v>
       </c>
-      <c r="L17">
+      <c r="L21">
         <v>1</v>
       </c>
-      <c r="M17">
+      <c r="M21">
         <v>71</v>
       </c>
-      <c r="N17">
+      <c r="N21">
         <v>256</v>
       </c>
-      <c r="O17">
+      <c r="O21" s="2">
         <v>10</v>
       </c>
-      <c r="Q17" t="str">
+      <c r="Q21" t="str">
         <f t="shared" si="0"/>
         <v>{ 'stream' : 227, 'name' : 'zone1_consigne' ,'descr' : 'Consigne intérieure zone 1', 'byte1': 70, 'weight1': 1, 'byte2': 71, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C18">
-        <v>227</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C22">
+        <v>227</v>
+      </c>
+      <c r="D22" t="s">
         <v>11</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G22" t="s">
         <v>68</v>
       </c>
-      <c r="H18">
+      <c r="H22">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I22" t="s">
         <v>80</v>
       </c>
-      <c r="J18" t="str">
+      <c r="J22" t="str">
         <f t="shared" si="2"/>
         <v>Température ballon ECS milieu</v>
       </c>
-      <c r="K18">
+      <c r="K22">
         <v>108</v>
       </c>
-      <c r="L18">
+      <c r="L22">
         <v>1</v>
       </c>
-      <c r="M18">
+      <c r="M22">
         <v>109</v>
       </c>
-      <c r="N18">
+      <c r="N22">
         <v>256</v>
       </c>
-      <c r="O18">
+      <c r="O22" s="2">
         <v>10</v>
       </c>
-      <c r="Q18" t="str">
+      <c r="Q22" t="str">
         <f t="shared" si="0"/>
         <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_milieu' ,'descr' : 'Température ballon ECS milieu', 'byte1': 108, 'weight1': 1, 'byte2': 109, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B23" t="s">
         <v>50</v>
       </c>
-      <c r="C19">
-        <v>227</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C23">
+        <v>227</v>
+      </c>
+      <c r="D23" t="s">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G23" t="s">
         <v>68</v>
       </c>
-      <c r="H19">
+      <c r="H23">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I23" t="s">
         <v>81</v>
       </c>
-      <c r="J19" t="str">
+      <c r="J23" t="str">
         <f t="shared" si="2"/>
         <v>Température ballon ECS bas</v>
       </c>
-      <c r="K19">
+      <c r="K23">
         <v>110</v>
       </c>
-      <c r="L19">
+      <c r="L23">
         <v>1</v>
       </c>
-      <c r="M19">
+      <c r="M23">
         <v>111</v>
       </c>
-      <c r="N19">
+      <c r="N23">
         <v>256</v>
       </c>
-      <c r="O19">
+      <c r="O23" s="2">
         <v>10</v>
       </c>
-      <c r="Q19" t="str">
+      <c r="Q23" t="str">
         <f t="shared" si="0"/>
         <v>{ 'stream' : 227, 'name' : 'ecs_temp_eau_bas' ,'descr' : 'Température ballon ECS bas', 'byte1': 110, 'weight1': 1, 'byte2': 111, 'weight2': 256, 'divider': 10 },</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
-        <v>250</v>
-      </c>
-      <c r="C20">
-        <v>227</v>
-      </c>
-      <c r="D20" t="s">
-        <v>252</v>
-      </c>
-      <c r="G20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
-        <v>227</v>
-      </c>
-      <c r="I20" t="s">
-        <v>251</v>
-      </c>
-      <c r="J20" t="s">
-        <v>250</v>
-      </c>
-      <c r="K20">
-        <v>122</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>123</v>
-      </c>
-      <c r="N20">
-        <v>256</v>
-      </c>
-      <c r="O20">
-        <v>10</v>
-      </c>
-      <c r="Q20" t="str">
-        <f t="shared" si="0"/>
-        <v>{ 'stream' : 227, 'name' : 'ecs_consigne' ,'descr' : 'Température consigne ECS', 'byte1': 122, 'weight1': 1, 'byte2': 123, 'weight2': 256, 'divider': 10 },</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21">
-        <v>227</v>
-      </c>
-      <c r="E21">
-        <v>168</v>
-      </c>
-      <c r="G21" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="1"/>
-        <v>227</v>
-      </c>
-      <c r="I21" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="2"/>
-        <v>Date année</v>
-      </c>
-      <c r="Q21" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22">
-        <v>227</v>
-      </c>
-      <c r="E22">
-        <v>169</v>
-      </c>
-      <c r="G22" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
-        <v>227</v>
-      </c>
-      <c r="I22" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" t="str">
-        <f t="shared" si="2"/>
-        <v>Date mois</v>
-      </c>
-      <c r="Q22" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23">
-        <v>227</v>
-      </c>
-      <c r="E23">
-        <v>170</v>
-      </c>
-      <c r="G23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
-        <v>227</v>
-      </c>
-      <c r="I23" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" t="str">
-        <f t="shared" si="2"/>
-        <v>Date jour</v>
-      </c>
-      <c r="Q23" t="str">
-        <f t="shared" si="0"/>
-        <v/>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>249</v>
       </c>
       <c r="C24">
         <v>227</v>
       </c>
-      <c r="E24">
-        <v>171</v>
+      <c r="D24" t="s">
+        <v>251</v>
       </c>
       <c r="G24" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I24" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" si="2"/>
-        <v>Date heure</v>
+        <v>250</v>
+      </c>
+      <c r="J24" t="s">
+        <v>249</v>
+      </c>
+      <c r="K24">
+        <v>122</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>123</v>
+      </c>
+      <c r="N24">
+        <v>256</v>
+      </c>
+      <c r="O24" s="2">
+        <v>10</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>{ 'stream' : 227, 'name' : 'ecs_consigne' ,'descr' : 'Température consigne ECS', 'byte1': 122, 'weight1': 1, 'byte2': 123, 'weight2': 256, 'divider': 10 },</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
@@ -2332,27 +2459,42 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>289</v>
       </c>
       <c r="C25">
         <v>227</v>
       </c>
-      <c r="E25">
-        <v>172</v>
+      <c r="D25" t="s">
+        <v>283</v>
       </c>
       <c r="G25" t="s">
-        <v>53</v>
+        <v>288</v>
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I25" t="s">
-        <v>53</v>
+        <v>284</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="2"/>
-        <v>Date minutes</v>
+        <f>B25</f>
+        <v>Nombre de cycles compresseur ? Geotwin ?</v>
+      </c>
+      <c r="K25">
+        <v>147</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>148</v>
+      </c>
+      <c r="N25">
+        <v>256</v>
+      </c>
+      <c r="O25" s="2">
+        <v>1</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="0"/>
@@ -2364,13 +2506,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <v>227</v>
       </c>
       <c r="E26">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G26" t="s">
         <v>53</v>
@@ -2384,7 +2526,7 @@
       </c>
       <c r="J26" t="str">
         <f t="shared" si="2"/>
-        <v>Date secondes</v>
+        <v>Date année</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="0"/>
@@ -2396,54 +2538,62 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>227</v>
       </c>
+      <c r="E27">
+        <v>169</v>
+      </c>
       <c r="G27" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I27" t="s">
-        <v>144</v>
-      </c>
-      <c r="J27" t="s">
-        <v>143</v>
-      </c>
-      <c r="K27">
-        <v>193</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="2"/>
+        <v>Date mois</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C28">
         <v>227</v>
+      </c>
+      <c r="E28">
+        <v>170</v>
+      </c>
+      <c r="G28" t="s">
+        <v>53</v>
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="J28" t="str">
-        <f>B28</f>
-        <v>Mode zone 1</v>
+        <f t="shared" si="2"/>
+        <v>Date jour</v>
       </c>
       <c r="Q28" t="str">
-        <f>IF(G28="Oui",_xlfn.CONCAT("{ 'stream' : ",H28,", 'name' : '",I28,"' ,'descr' : '",J28,"', 'byte1': ",K28,", 'weight1': ",L28,", 'byte2': ",M28,", 'weight2': ",N28,", 'divider': ",O28," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2452,160 +2602,327 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="C29">
+        <v>227</v>
+      </c>
+      <c r="E29">
+        <v>171</v>
+      </c>
+      <c r="G29" t="s">
+        <v>53</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="I29" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="J29" t="str">
-        <f>B29</f>
-        <v>Marche/Arrêt Général</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>Date heure</v>
       </c>
       <c r="Q29" t="str">
-        <f>IF(G29="Oui",_xlfn.CONCAT("{ 'stream' : ",H29,", 'name' : '",I29,"' ,'descr' : '",J29,"', 'byte1': ",K29,", 'weight1': ",L29,", 'byte2': ",M29,", 'weight2': ",N29,", 'divider': ",O29," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>227</v>
+      </c>
+      <c r="E30">
+        <v>172</v>
+      </c>
+      <c r="G30" t="s">
+        <v>53</v>
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="I30" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="J30" t="str">
-        <f>B30</f>
-        <v>Température eau départ zone 1</v>
+        <f t="shared" si="2"/>
+        <v>Date minutes</v>
       </c>
       <c r="Q30" t="str">
-        <f>IF(G30="Oui",_xlfn.CONCAT("{ 'stream' : ",H30,", 'name' : '",I30,"' ,'descr' : '",J30,"', 'byte1': ",K30,", 'weight1': ",L30,", 'byte2': ",M30,", 'weight2': ",N30,", 'divider': ",O30," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>227</v>
+      </c>
+      <c r="E31">
+        <v>173</v>
+      </c>
+      <c r="G31" t="s">
+        <v>53</v>
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="I31" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="J31" t="str">
-        <f>B31</f>
-        <v>Température eau retour zone 1</v>
+        <f t="shared" si="2"/>
+        <v>Date secondes</v>
       </c>
       <c r="Q31" t="str">
-        <f>IF(G31="Oui",_xlfn.CONCAT("{ 'stream' : ",H31,", 'name' : '",I31,"' ,'descr' : '",J31,"', 'byte1': ",K31,", 'weight1': ",L31,", 'byte2': ",M31,", 'weight2': ",N31,", 'divider': ",O31," }," ),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>142</v>
+      </c>
+      <c r="C32">
+        <v>227</v>
+      </c>
+      <c r="G32" t="s">
+        <v>110</v>
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="I32" t="s">
-        <v>79</v>
-      </c>
-      <c r="J32" t="str">
-        <f>B32</f>
-        <v>Etat (marche)</v>
-      </c>
-      <c r="Q32" t="str">
-        <f>IF(G32="Oui",_xlfn.CONCAT("{ 'stream' : ",H32,", 'name' : '",I32,"' ,'descr' : '",J32,"', 'byte1': ",K32,", 'weight1': ",L32,", 'byte2': ",M32,", 'weight2': ",N32,", 'divider': ",O32," }," ),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+      <c r="J32" t="s">
+        <v>142</v>
+      </c>
+      <c r="K32">
+        <v>193</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="C33">
+        <v>227</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>227</v>
+      </c>
+      <c r="I33" t="s">
+        <v>73</v>
+      </c>
+      <c r="J33" t="str">
+        <f>B33</f>
+        <v>Mode zone 1</v>
+      </c>
+      <c r="Q33" t="str">
+        <f>IF(G33="Oui",_xlfn.CONCAT("{ 'stream' : ",H33,", 'name' : '",I33,"' ,'descr' : '",J33,"', 'byte1': ",K33,", 'weight1': ",L33,", 'byte2': ",M33,", 'weight2': ",N33,", 'divider': ",O33," }," ),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>69</v>
+      </c>
+      <c r="J34" t="str">
+        <f>B34</f>
+        <v>Marche/Arrêt Général</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="str">
+        <f>IF(G34="Oui",_xlfn.CONCAT("{ 'stream' : ",H34,", 'name' : '",I34,"' ,'descr' : '",J34,"', 'byte1': ",K34,", 'weight1': ",L34,", 'byte2': ",M34,", 'weight2': ",N34,", 'divider': ",O34," }," ),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>9</v>
       </c>
       <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>76</v>
+      </c>
+      <c r="J35" t="str">
+        <f>B35</f>
+        <v>Température eau départ zone 1</v>
+      </c>
+      <c r="Q35" t="str">
+        <f>IF(G35="Oui",_xlfn.CONCAT("{ 'stream' : ",H35,", 'name' : '",I35,"' ,'descr' : '",J35,"', 'byte1': ",K35,", 'weight1': ",L35,", 'byte2': ",M35,", 'weight2': ",N35,", 'divider': ",O35," }," ),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>77</v>
+      </c>
+      <c r="J36" t="str">
+        <f>B36</f>
+        <v>Température eau retour zone 1</v>
+      </c>
+      <c r="Q36" t="str">
+        <f>IF(G36="Oui",_xlfn.CONCAT("{ 'stream' : ",H36,", 'name' : '",I36,"' ,'descr' : '",J36,"', 'byte1': ",K36,", 'weight1': ",L36,", 'byte2': ",M36,", 'weight2': ",N36,", 'divider': ",O36," }," ),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>79</v>
+      </c>
+      <c r="J37" t="str">
+        <f>B37</f>
+        <v>Etat (marche)</v>
+      </c>
+      <c r="Q37" t="str">
+        <f>IF(G37="Oui",_xlfn.CONCAT("{ 'stream' : ",H37,", 'name' : '",I37,"' ,'descr' : '",J37,"', 'byte1': ",K37,", 'weight1': ",L37,", 'byte2': ",M37,", 'weight2': ",N37,", 'divider': ",O37," }," ),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>7</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B42" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>7</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B43" t="s">
         <v>89</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E43" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>287</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q32">
-    <sortCondition ref="C2:C32"/>
-    <sortCondition ref="K2:K32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q37">
+    <sortCondition ref="C2:C37"/>
+    <sortCondition ref="K2:K37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2616,8 +2933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA0E6119-EB0F-4A94-9FD9-76ECAE32D8E2}">
   <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="119" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView zoomScale="119" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2647,19 +2964,19 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="F1" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
       <c r="J1" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
       <c r="N1" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
@@ -2684,58 +3001,58 @@
         <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>38</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
@@ -2743,10 +3060,10 @@
         <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2755,7 +3072,7 @@
         <v>163</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H3" s="8">
         <v>12</v>
@@ -2781,14 +3098,14 @@
         <v/>
       </c>
       <c r="R3" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V3" s="10">
         <v>0</v>
@@ -2802,7 +3119,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2824,7 +3141,7 @@
         <v>156</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L4" s="9">
         <v>24</v>
@@ -2837,7 +3154,7 @@
         <v>156</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P4" s="8">
         <v>141</v>
@@ -2847,14 +3164,14 @@
         <v>129</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T4" s="10"/>
       <c r="U4" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V4" s="10">
         <v>12</v>
@@ -2865,10 +3182,10 @@
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2884,7 +3201,7 @@
         <v>156</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L5" s="9">
         <v>52</v>
@@ -2901,14 +3218,14 @@
         <v/>
       </c>
       <c r="R5" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T5" s="10"/>
       <c r="U5" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V5" s="10">
         <v>40</v>
@@ -2919,10 +3236,10 @@
         <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2938,7 +3255,7 @@
         <v>156</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L6" s="9">
         <v>54</v>
@@ -2955,14 +3272,14 @@
         <v/>
       </c>
       <c r="R6" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V6" s="10">
         <v>42</v>
@@ -2976,7 +3293,7 @@
         <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F7" s="8">
         <v>163</v>
@@ -3012,14 +3329,14 @@
         <v/>
       </c>
       <c r="R7" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T7" s="10"/>
       <c r="U7" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V7" s="10">
         <v>44</v>
@@ -3033,7 +3350,7 @@
         <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -3072,14 +3389,14 @@
         <v/>
       </c>
       <c r="R8" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T8" s="10"/>
       <c r="U8" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V8" s="10">
         <v>50</v>
@@ -3087,13 +3404,13 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" t="s">
         <v>247</v>
       </c>
-      <c r="B9" t="s">
-        <v>248</v>
-      </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -3102,7 +3419,7 @@
         <v>227</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H9" s="8">
         <v>12</v>
@@ -3123,16 +3440,16 @@
         <v/>
       </c>
       <c r="R9" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T9" s="10">
         <v>0</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V9" s="10">
         <v>0</v>
@@ -3143,10 +3460,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -3155,7 +3472,7 @@
         <v>227</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H10" s="8">
         <v>16</v>
@@ -3176,16 +3493,16 @@
         <v/>
       </c>
       <c r="R10" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T10" s="10">
         <v>4</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V10" s="10">
         <v>4</v>
@@ -3196,10 +3513,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -3208,7 +3525,7 @@
         <v>227</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H11" s="8">
         <v>18</v>
@@ -3229,16 +3546,16 @@
         <v/>
       </c>
       <c r="R11" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T11" s="10">
         <v>6</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V11" s="10">
         <v>6</v>
@@ -3249,10 +3566,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -3261,7 +3578,7 @@
         <v>227</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H12" s="8">
         <v>30</v>
@@ -3287,16 +3604,16 @@
         <v/>
       </c>
       <c r="R12" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T12" s="10">
         <v>18</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V12" s="10">
         <v>18</v>
@@ -3310,7 +3627,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D13">
         <v>54.55</v>
@@ -3335,7 +3652,7 @@
         <v>220</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L13" s="9">
         <v>54</v>
@@ -3348,7 +3665,7 @@
         <v>150</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P13" s="8">
         <v>55</v>
@@ -3358,16 +3675,16 @@
         <v>13</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S13" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="T13" s="10">
+        <v>2</v>
+      </c>
+      <c r="U13" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="T13" s="10">
-        <v>2</v>
-      </c>
-      <c r="U13" s="10" t="s">
-        <v>225</v>
       </c>
       <c r="V13" s="10">
         <v>42</v>
@@ -3381,7 +3698,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D14">
         <v>56.57</v>
@@ -3406,7 +3723,7 @@
         <v>220</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L14" s="9">
         <v>56</v>
@@ -3419,7 +3736,7 @@
         <v>150</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P14" s="8">
         <v>57</v>
@@ -3429,16 +3746,16 @@
         <v>13</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T14" s="10">
         <v>4</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V14" s="10">
         <v>44</v>
@@ -3452,7 +3769,7 @@
         <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -3474,7 +3791,7 @@
         <v>220</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L15" s="9">
         <v>62</v>
@@ -3487,7 +3804,7 @@
         <v>150</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P15" s="8">
         <v>81</v>
@@ -3497,16 +3814,16 @@
         <v>31</v>
       </c>
       <c r="R15" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T15" s="10">
         <v>10</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V15" s="10">
         <v>50</v>
@@ -3520,7 +3837,7 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -3542,7 +3859,7 @@
         <v>220</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L16" s="9">
         <v>68</v>
@@ -3559,16 +3876,16 @@
         <v/>
       </c>
       <c r="R16" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T16" s="10">
         <v>0</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V16" s="10">
         <v>56</v>
@@ -3582,7 +3899,7 @@
         <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D17">
         <v>70.709999999999994</v>
@@ -3607,7 +3924,7 @@
         <v>220</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L17" s="9">
         <v>70</v>
@@ -3624,16 +3941,16 @@
         <v/>
       </c>
       <c r="R17" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="S17" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="S17" s="10" t="s">
-        <v>245</v>
-      </c>
       <c r="T17" s="10">
         <v>2</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V17" s="10">
         <v>58</v>
@@ -3644,10 +3961,10 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -3665,7 +3982,7 @@
         <v>220</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L18" s="9">
         <v>80</v>
@@ -3682,16 +3999,16 @@
         <v/>
       </c>
       <c r="R18" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T18" s="10">
         <v>14</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V18" s="10">
         <v>68</v>
@@ -3705,7 +4022,7 @@
         <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -3727,7 +4044,7 @@
         <v>220</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L19" s="9">
         <v>108</v>
@@ -3740,7 +4057,7 @@
         <v>150</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P19" s="8">
         <v>71</v>
@@ -3750,16 +4067,16 @@
         <v>-25</v>
       </c>
       <c r="R19" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T19" s="10">
         <v>0</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V19" s="10">
         <v>96</v>
@@ -3773,7 +4090,7 @@
         <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -3795,7 +4112,7 @@
         <v>220</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L20" s="9">
         <v>110</v>
@@ -3808,7 +4125,7 @@
         <v>150</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P20" s="8">
         <v>73</v>
@@ -3818,16 +4135,16 @@
         <v>-25</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T20" s="10">
         <v>2</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V20" s="10">
         <v>98</v>
@@ -3838,19 +4155,19 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="8">
+        <v>227</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="C21" t="s">
-        <v>142</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21" s="8">
-        <v>227</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="H21" s="8">
         <v>122</v>
@@ -3868,16 +4185,16 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T21" s="10">
         <v>14</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V21" s="10">
         <v>110</v>
@@ -3888,10 +4205,10 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22" s="8">
         <v>227</v>
@@ -3906,7 +4223,7 @@
         <v>220</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L22" s="9">
         <v>178</v>
@@ -3936,7 +4253,7 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D23">
         <v>168</v>
@@ -3984,7 +4301,7 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D24">
         <v>169</v>
@@ -4032,7 +4349,7 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D25">
         <v>170</v>
@@ -4080,7 +4397,7 @@
         <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D26">
         <v>171</v>
@@ -4128,7 +4445,7 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D27">
         <v>172</v>
@@ -4176,7 +4493,7 @@
         <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D28">
         <v>173</v>
@@ -4224,7 +4541,7 @@
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F29" s="8">
         <v>227</v>
@@ -4264,16 +4581,16 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="8">
+        <v>227</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="C30" t="s">
-        <v>142</v>
-      </c>
-      <c r="F30" s="8">
-        <v>227</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>144</v>
       </c>
       <c r="H30" s="8">
         <v>193</v>
@@ -4286,7 +4603,7 @@
         <v>220</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L30" s="9">
         <v>193</v>
@@ -4527,7 +4844,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4540,18 +4857,18 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -4559,7 +4876,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G3" s="16">
         <v>1</v>
@@ -4570,19 +4887,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G6" s="16">
         <v>1</v>
@@ -4593,31 +4910,31 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -4628,7 +4945,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -4640,7 +4957,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -4652,7 +4969,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -4664,7 +4981,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -4676,7 +4993,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G16" s="16">
         <v>1</v>
@@ -4684,19 +5001,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19">
@@ -4705,7 +5022,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G20">
         <v>4</v>
@@ -4716,7 +5033,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G21">
         <v>2</v>
@@ -4728,7 +5045,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G22">
         <v>10</v>
@@ -4740,7 +5057,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G23">
         <v>4</v>
@@ -4752,7 +5069,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -4764,7 +5081,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -4776,7 +5093,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -4784,7 +5101,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H29">
         <v>40</v>
@@ -4792,7 +5109,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H30">
         <v>42</v>
@@ -4800,7 +5117,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H31">
         <v>44</v>
@@ -4808,7 +5125,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H32">
         <v>46</v>
@@ -4816,7 +5133,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H33">
         <v>48</v>
@@ -4824,7 +5141,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H34">
         <v>50</v>
@@ -4832,7 +5149,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H35">
         <v>52</v>
@@ -4840,7 +5157,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H36">
         <v>53</v>
@@ -4848,7 +5165,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H37">
         <v>54</v>
@@ -4856,7 +5173,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B38">
         <v>40</v>
@@ -4864,7 +5181,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H39">
         <v>56</v>
@@ -4872,7 +5189,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H40">
         <v>58</v>
@@ -4880,12 +5197,12 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H42">
         <v>68</v>
@@ -4893,12 +5210,12 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B44">
         <v>16</v>
@@ -4909,7 +5226,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H45">
         <v>96</v>
@@ -4917,7 +5234,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H46">
         <v>98</v>
@@ -4925,7 +5242,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H47">
         <v>100</v>
@@ -4933,12 +5250,12 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H49">
         <v>110</v>
@@ -4959,7 +5276,7 @@
   <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="D16" sqref="D16:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4975,58 +5292,58 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" t="s">
         <v>165</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>164</v>
       </c>
-      <c r="K1" t="s">
-        <v>166</v>
-      </c>
-      <c r="O1" t="s">
-        <v>165</v>
-      </c>
       <c r="Q1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2">
         <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3">
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N3">
         <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -5035,10 +5352,10 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O4">
         <v>10</v>
@@ -5049,7 +5366,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -5058,7 +5375,7 @@
         <v>10</v>
       </c>
       <c r="N5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O5">
         <v>2</v>
@@ -5069,7 +5386,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -5078,7 +5395,7 @@
         <v>12</v>
       </c>
       <c r="N6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O6">
         <v>2</v>
@@ -5089,7 +5406,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -5098,7 +5415,7 @@
         <v>14</v>
       </c>
       <c r="N7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O7">
         <v>2</v>
@@ -5109,7 +5426,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -5118,7 +5435,7 @@
         <v>16</v>
       </c>
       <c r="N8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O8">
         <v>2</v>
@@ -5129,7 +5446,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -5138,7 +5455,7 @@
         <v>18</v>
       </c>
       <c r="N9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O9">
         <v>2</v>
@@ -5149,7 +5466,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -5158,7 +5475,7 @@
         <v>22</v>
       </c>
       <c r="N10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O10">
         <v>4</v>
@@ -5169,13 +5486,13 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11">
         <v>124</v>
       </c>
       <c r="M11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N11">
         <v>124</v>
@@ -5183,16 +5500,16 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D12">
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O12">
         <v>32</v>
@@ -5200,7 +5517,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -5209,7 +5526,7 @@
         <v>24</v>
       </c>
       <c r="N13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O13">
         <v>20</v>
@@ -5217,7 +5534,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -5226,7 +5543,7 @@
         <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O14">
         <v>9</v>
@@ -5234,7 +5551,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -5245,7 +5562,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -5256,7 +5573,7 @@
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -5267,7 +5584,7 @@
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -5278,7 +5595,7 @@
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -5289,7 +5606,7 @@
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -5300,7 +5617,7 @@
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -5311,7 +5628,7 @@
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -5322,7 +5639,7 @@
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F23">
         <v>2</v>
@@ -5333,7 +5650,7 @@
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -5344,7 +5661,7 @@
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -5355,7 +5672,7 @@
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F26">
         <v>2</v>
@@ -5366,7 +5683,7 @@
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -5377,7 +5694,7 @@
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F28">
         <v>2</v>
@@ -5388,7 +5705,7 @@
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -5399,7 +5716,7 @@
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F30">
         <v>2</v>
@@ -5410,7 +5727,7 @@
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -5421,7 +5738,7 @@
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F32">
         <v>2</v>
@@ -5432,7 +5749,7 @@
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -5443,7 +5760,7 @@
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -5454,7 +5771,7 @@
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F35">
         <v>2</v>
@@ -5465,7 +5782,7 @@
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F36">
         <v>2</v>
@@ -5476,7 +5793,7 @@
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D37">
         <v>12</v>
@@ -5487,7 +5804,7 @@
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -5498,7 +5815,7 @@
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -5509,7 +5826,7 @@
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D45">
         <v>8</v>
@@ -5520,7 +5837,7 @@
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D46">
         <v>8</v>
@@ -5545,37 +5862,37 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3">
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -5586,7 +5903,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -5598,7 +5915,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -5610,7 +5927,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -5622,7 +5939,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -5634,7 +5951,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -5646,7 +5963,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -5658,7 +5975,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11">
         <v>124</v>
@@ -5669,7 +5986,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D12">
         <v>32</v>
@@ -5680,7 +5997,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D13">
         <v>20</v>
@@ -5691,7 +6008,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D14">
         <v>8</v>
@@ -5702,7 +6019,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -5713,7 +6030,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -5724,7 +6041,7 @@
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -5735,7 +6052,7 @@
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -5746,7 +6063,7 @@
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D19">
         <v>8</v>

</xml_diff>